<commit_message>
Oppdatert regneark, lagt inn slettede journaler, slettede postjournaler og noen midre barnvernsfaglige logikkendringer.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2569" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D129DD5-84E1-4F93-884E-0741F59D12D8}"/>
+  <xr:revisionPtr revIDLastSave="2662" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED68B2E4-EAAE-465F-9BA6-9A82D52BD650}"/>
   <bookViews>
-    <workbookView xWindow="6850" yWindow="2120" windowWidth="28300" windowHeight="17380" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="1380" windowWidth="27250" windowHeight="17380" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4815" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4817" uniqueCount="966">
   <si>
     <t>Format</t>
   </si>
@@ -2444,33 +2444,6 @@
     <t>FA_JOURNAL.JOU_LOEPENR+&lt;BYDELSNUMMER&gt;</t>
   </si>
   <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_KLIENT.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_MELDINGER.Mel_Loepenr+&lt;BYDELSNUMMER&gt; + "SAK-MUS"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_KLIENTTILKNYTNING.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_MELDINGER.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_UNDERSØKELSE.FA_MELDING.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_SAKSJOURNAL.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_TILTAK.KLI_LOPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_TILTAKSPLAN.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_POSTJOURNAL.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
-  </si>
-  <si>
     <t>FA_FORBINDELSER.FOR_LOEPENR+&lt;BYDELSNUMMER&gt;+"FOR"</t>
   </si>
   <si>
@@ -2508,9 +2481,6 @@
   </si>
   <si>
     <t>FA_JOURNAL.JOU_LOEPENR+&lt;BYDELSNUMMER&gt;+"JOU"</t>
-  </si>
-  <si>
-    <t>ÅÅÅÅ(Kli_Registrertdato) + FA_JOURNAL.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
   </si>
   <si>
     <t>SAMLENOTAT</t>
@@ -2834,9 +2804,6 @@
     <t>SuppliersAndContractorsTeam</t>
   </si>
   <si>
-    <t>ÅÅÅÅ(Med_Registrertdato) + FA_MEDARBEIDERE.FOR_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK-OPP"</t>
-  </si>
-  <si>
     <t>Unik ID til brukeren (BrukerId) som godkjente vedtaket. Feltet kan kun angis dersom Status=UTFØRT. Dersom Status=UTFØRT, men feltet ikke er angitt, så benyttes samme verdi som SaksbehandlerId.</t>
   </si>
   <si>
@@ -2915,9 +2882,6 @@
     <t>FA_SAKSJOURNAL med samme FA_UNDERSOEKELSE.MEL_LOEPENR</t>
   </si>
   <si>
-    <t>Utvidelse av frist</t>
-  </si>
-  <si>
     <t>FA_UNDERSOEKELSE.MEL_LOEPENR+&lt;BYDELSNUMMER&gt;+"UNDUT"</t>
   </si>
   <si>
@@ -2946,6 +2910,66 @@
   </si>
   <si>
     <t>FA_JOURNAL SLETTET</t>
+  </si>
+  <si>
+    <t>FA_UNDERSOEKELSE.UND_FRISTDATO - 90 dager</t>
+  </si>
+  <si>
+    <t>FA_UNDERSOEKELSE.UND_6MNDBEGRUNNELSE</t>
+  </si>
+  <si>
+    <t>Utvidelse av frist (lage tekst-dokument med Notat-feltet)</t>
+  </si>
+  <si>
+    <t>FA_UNDERSOEKELSE.SBH_INITIALER</t>
+  </si>
+  <si>
+    <t>Beslutning om utvidet undersøkelsestid</t>
+  </si>
+  <si>
+    <t>Frist for gjennomføring av undersøkelsen</t>
+  </si>
+  <si>
+    <t>Utvidet frist</t>
+  </si>
+  <si>
+    <t>FA_KLIENT.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_MELDINGER.Mel_Loepenr+&lt;BYDELSNUMMER&gt; + "SAK-MUS"</t>
+  </si>
+  <si>
+    <t>FA_MEDARBEIDERE.FOR_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK-OPP"</t>
+  </si>
+  <si>
+    <t>FA_KLIENTTILKNYTNING.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_MELDINGER.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_UNDERSØKELSE.FA_MELDING.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_SAKSJOURNAL.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_TILTAK.KLI_LOPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_TILTAKSPLAN.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_POSTJOURNAL.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_JOURNAL.KLI_LOEPENR+&lt;BYDELSNUMMER&gt; + "SAK"</t>
+  </si>
+  <si>
+    <t>FA_UNDERSOEKELSE.FRO_KODE1, FRO_KODE2 og FRO_KODE3 (Bruk 30_ANNET_(BRUK_GJERNE_STIKKORD) hvis ikke utfylt)</t>
+  </si>
+  <si>
+    <t>Hvis 30_ANNET_(BRUK_GJERNE_STIKKORD) -&gt; FA_UNDERSOEKELSE.UND_6MNDBEGRUNNELSE</t>
   </si>
 </sst>
 </file>
@@ -3101,7 +3125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3255,11 +3279,8 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3588,7 +3609,9 @@
   </sheetPr>
   <dimension ref="A1:W928"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A843" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A848" sqref="A848"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3966,7 +3989,7 @@
         <v>589</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>791</v>
+        <v>953</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
@@ -3986,7 +4009,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>926</v>
+        <v>915</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>32</v>
@@ -4118,7 +4141,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>422</v>
@@ -4132,7 +4155,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>20</v>
@@ -4160,7 +4183,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>927</v>
+        <v>916</v>
       </c>
       <c r="G25" s="41" t="s">
         <v>439</v>
@@ -4308,13 +4331,13 @@
     </row>
     <row r="36" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="45" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>20</v>
@@ -4322,13 +4345,13 @@
     </row>
     <row r="37" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="45" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>20</v>
@@ -4342,7 +4365,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>20</v>
@@ -4382,7 +4405,7 @@
         <v>589</v>
       </c>
       <c r="G40" s="41" t="s">
-        <v>792</v>
+        <v>954</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -4402,7 +4425,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>926</v>
+        <v>915</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>759</v>
@@ -4534,7 +4557,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="G48" s="41" t="s">
         <v>763</v>
@@ -4548,7 +4571,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>20</v>
@@ -4576,7 +4599,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>927</v>
+        <v>916</v>
       </c>
       <c r="G51" s="41" t="s">
         <v>439</v>
@@ -4724,13 +4747,13 @@
     </row>
     <row r="62" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="45" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>20</v>
@@ -4738,13 +4761,13 @@
     </row>
     <row r="63" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="45" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="G63" s="6" t="s">
         <v>20</v>
@@ -4758,7 +4781,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>20</v>
@@ -4798,7 +4821,7 @@
         <v>589</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>791</v>
+        <v>953</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -4818,7 +4841,7 @@
         <v>50</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>926</v>
+        <v>915</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>32</v>
@@ -4950,7 +4973,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>422</v>
@@ -4964,7 +4987,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>20</v>
@@ -4992,7 +5015,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>927</v>
+        <v>916</v>
       </c>
       <c r="G77" s="41" t="s">
         <v>617</v>
@@ -5140,13 +5163,13 @@
     </row>
     <row r="88" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="45" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="C88" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>20</v>
@@ -5154,13 +5177,13 @@
     </row>
     <row r="89" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="45" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="C89" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>20</v>
@@ -5174,7 +5197,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>20</v>
@@ -5214,7 +5237,7 @@
         <v>589</v>
       </c>
       <c r="G92" s="41" t="s">
-        <v>920</v>
+        <v>955</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -5234,10 +5257,10 @@
         <v>50</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>926</v>
+        <v>915</v>
       </c>
       <c r="G93" s="41" t="s">
-        <v>919</v>
+        <v>909</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -5260,7 +5283,7 @@
         <v>278</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>928</v>
+        <v>917</v>
       </c>
       <c r="H94" s="28" t="s">
         <v>180</v>
@@ -5366,7 +5389,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>772</v>
@@ -5380,7 +5403,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>20</v>
@@ -5408,7 +5431,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>927</v>
+        <v>916</v>
       </c>
       <c r="G103" s="41" t="s">
         <v>774</v>
@@ -5556,13 +5579,13 @@
     </row>
     <row r="114" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="45" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="C114" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="G114" s="6" t="s">
         <v>20</v>
@@ -5570,13 +5593,13 @@
     </row>
     <row r="115" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="45" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="C115" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="G115" s="6" t="s">
         <v>20</v>
@@ -5590,7 +5613,7 @@
         <v>1</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>20</v>
@@ -5870,7 +5893,7 @@
         <v>5</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="G134" s="6" t="s">
         <v>20</v>
@@ -6542,7 +6565,7 @@
         <v>5</v>
       </c>
       <c r="F180" s="6" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="G180" s="6" t="s">
         <v>20</v>
@@ -6977,7 +7000,7 @@
         <v>680</v>
       </c>
       <c r="G210" s="6" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="211" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -7216,7 +7239,7 @@
         <v>5</v>
       </c>
       <c r="F226" s="6" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="G226" s="41" t="s">
         <v>630</v>
@@ -7651,7 +7674,7 @@
         <v>681</v>
       </c>
       <c r="G256" s="6" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="257" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -7755,7 +7778,7 @@
         <v>578</v>
       </c>
       <c r="G263" s="6" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="264" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -8034,7 +8057,7 @@
         <v>34</v>
       </c>
       <c r="G282" s="20" t="s">
-        <v>791</v>
+        <v>953</v>
       </c>
       <c r="H282" s="9"/>
     </row>
@@ -8142,7 +8165,7 @@
         <v>34</v>
       </c>
       <c r="G289" s="23" t="s">
-        <v>793</v>
+        <v>956</v>
       </c>
       <c r="H289" s="9"/>
     </row>
@@ -8160,7 +8183,7 @@
         <v>107</v>
       </c>
       <c r="G290" s="23" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="H290" s="9"/>
     </row>
@@ -8606,7 +8629,7 @@
         <v>208</v>
       </c>
       <c r="G307" s="42" t="s">
-        <v>894</v>
+        <v>884</v>
       </c>
       <c r="H307" s="9"/>
       <c r="I307" s="5"/>
@@ -8725,7 +8748,7 @@
         <v>34</v>
       </c>
       <c r="G312" s="23" t="s">
-        <v>794</v>
+        <v>957</v>
       </c>
       <c r="H312" s="27"/>
     </row>
@@ -8745,7 +8768,7 @@
         <v>755</v>
       </c>
       <c r="G313" s="20" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="H313" s="27"/>
     </row>
@@ -9196,7 +9219,7 @@
         <v>754</v>
       </c>
       <c r="G342" s="41" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
     </row>
     <row r="343" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -9410,7 +9433,7 @@
         <v>752</v>
       </c>
       <c r="G356" s="41" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
     </row>
     <row r="357" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
@@ -9516,7 +9539,7 @@
         <v>631</v>
       </c>
       <c r="G362" s="33" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="H362" s="9"/>
     </row>
@@ -9534,7 +9557,7 @@
         <v>210</v>
       </c>
       <c r="G363" s="33" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="H363" s="9"/>
     </row>
@@ -9552,7 +9575,7 @@
         <v>34</v>
       </c>
       <c r="G364" s="20" t="s">
-        <v>795</v>
+        <v>958</v>
       </c>
       <c r="H364" s="9"/>
     </row>
@@ -9888,7 +9911,7 @@
         <v>744</v>
       </c>
       <c r="G384" s="33" t="s">
-        <v>946</v>
+        <v>935</v>
       </c>
       <c r="H384" s="9"/>
     </row>
@@ -10041,7 +10064,7 @@
         <v>751</v>
       </c>
       <c r="G393" s="33" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="H393" s="9"/>
     </row>
@@ -10059,7 +10082,7 @@
         <v>34</v>
       </c>
       <c r="G394" s="42" t="s">
-        <v>796</v>
+        <v>959</v>
       </c>
       <c r="H394" s="9"/>
     </row>
@@ -10086,7 +10109,7 @@
         <v>1</v>
       </c>
       <c r="F396" s="6" t="s">
-        <v>921</v>
+        <v>910</v>
       </c>
       <c r="G396" s="33" t="s">
         <v>718</v>
@@ -10104,7 +10127,7 @@
         <v>1</v>
       </c>
       <c r="F397" s="6" t="s">
-        <v>893</v>
+        <v>883</v>
       </c>
       <c r="G397" s="33" t="s">
         <v>306</v>
@@ -10137,7 +10160,7 @@
         <v>12</v>
       </c>
       <c r="F399" s="6" t="s">
-        <v>922</v>
+        <v>911</v>
       </c>
       <c r="G399" s="33" t="s">
         <v>720</v>
@@ -10152,7 +10175,7 @@
         <v>12</v>
       </c>
       <c r="F400" s="6" t="s">
-        <v>923</v>
+        <v>912</v>
       </c>
       <c r="G400" s="33" t="s">
         <v>721</v>
@@ -10167,7 +10190,7 @@
         <v>1</v>
       </c>
       <c r="F401" s="6" t="s">
-        <v>924</v>
+        <v>913</v>
       </c>
       <c r="G401" s="33" t="s">
         <v>307</v>
@@ -10182,7 +10205,7 @@
         <v>12</v>
       </c>
       <c r="F402" s="6" t="s">
-        <v>925</v>
+        <v>914</v>
       </c>
       <c r="G402" s="33" t="s">
         <v>721</v>
@@ -10335,7 +10358,7 @@
         <v>225</v>
       </c>
       <c r="G412" s="33" t="s">
-        <v>936</v>
+        <v>925</v>
       </c>
       <c r="H412" s="9"/>
     </row>
@@ -10554,7 +10577,7 @@
         <v>598</v>
       </c>
       <c r="G426" s="33" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
       <c r="H426" s="9"/>
     </row>
@@ -10572,7 +10595,7 @@
         <v>34</v>
       </c>
       <c r="G427" s="33" t="s">
-        <v>797</v>
+        <v>960</v>
       </c>
       <c r="H427" s="9"/>
     </row>
@@ -10590,7 +10613,7 @@
         <v>233</v>
       </c>
       <c r="G428" s="33" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="H428" s="9"/>
     </row>
@@ -10874,7 +10897,7 @@
         <v>1</v>
       </c>
       <c r="G446" s="33" t="s">
-        <v>912</v>
+        <v>902</v>
       </c>
       <c r="H446" s="9"/>
     </row>
@@ -10886,10 +10909,10 @@
         <v>1</v>
       </c>
       <c r="F447" s="6" t="s">
-        <v>909</v>
+        <v>899</v>
       </c>
       <c r="G447" s="33" t="s">
-        <v>913</v>
+        <v>903</v>
       </c>
       <c r="H447" s="9"/>
     </row>
@@ -10901,10 +10924,10 @@
         <v>1</v>
       </c>
       <c r="F448" s="6" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="G448" s="33" t="s">
-        <v>914</v>
+        <v>904</v>
       </c>
       <c r="H448" s="9"/>
     </row>
@@ -10916,7 +10939,7 @@
         <v>1</v>
       </c>
       <c r="F449" s="6" t="s">
-        <v>907</v>
+        <v>897</v>
       </c>
       <c r="G449" s="33" t="s">
         <v>20</v>
@@ -10949,7 +10972,7 @@
         <v>597</v>
       </c>
       <c r="G451" s="33" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="H451" s="9"/>
     </row>
@@ -10967,7 +10990,7 @@
         <v>579</v>
       </c>
       <c r="G452" s="23" t="s">
-        <v>798</v>
+        <v>961</v>
       </c>
       <c r="H452" s="9"/>
     </row>
@@ -11658,7 +11681,7 @@
         <v>756</v>
       </c>
       <c r="G498" s="20" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="H498" s="9"/>
       <c r="I498" s="5"/>
@@ -11691,7 +11714,7 @@
         <v>34</v>
       </c>
       <c r="G499" s="20" t="s">
-        <v>799</v>
+        <v>962</v>
       </c>
       <c r="H499" s="9"/>
       <c r="I499" s="5"/>
@@ -12487,7 +12510,7 @@
         <v>756</v>
       </c>
       <c r="G525" s="20" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="H525" s="9"/>
       <c r="I525" s="5"/>
@@ -12520,7 +12543,7 @@
         <v>34</v>
       </c>
       <c r="G526" s="20" t="s">
-        <v>799</v>
+        <v>962</v>
       </c>
       <c r="H526" s="9"/>
       <c r="I526" s="5"/>
@@ -13316,7 +13339,7 @@
         <v>756</v>
       </c>
       <c r="G552" s="20" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="H552" s="9"/>
       <c r="I552" s="5"/>
@@ -13349,7 +13372,7 @@
         <v>34</v>
       </c>
       <c r="G553" s="20" t="s">
-        <v>799</v>
+        <v>962</v>
       </c>
       <c r="H553" s="9"/>
       <c r="I553" s="5"/>
@@ -14145,7 +14168,7 @@
         <v>756</v>
       </c>
       <c r="G579" s="33" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="H579" s="9"/>
       <c r="I579" s="5"/>
@@ -14178,7 +14201,7 @@
         <v>34</v>
       </c>
       <c r="G580" s="33" t="s">
-        <v>796</v>
+        <v>959</v>
       </c>
       <c r="H580" s="9"/>
       <c r="I580" s="5"/>
@@ -14914,7 +14937,7 @@
         <v>756</v>
       </c>
       <c r="G606" s="33" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="H606" s="9"/>
       <c r="I606" s="5"/>
@@ -14947,7 +14970,7 @@
         <v>34</v>
       </c>
       <c r="G607" s="33" t="s">
-        <v>813</v>
+        <v>963</v>
       </c>
       <c r="H607" s="9"/>
       <c r="I607" s="5"/>
@@ -14978,7 +15001,7 @@
         <v>430</v>
       </c>
       <c r="G608" s="20" t="s">
-        <v>814</v>
+        <v>804</v>
       </c>
       <c r="H608" s="9"/>
       <c r="I608" s="5"/>
@@ -15009,7 +15032,7 @@
         <v>430</v>
       </c>
       <c r="G609" s="42" t="s">
-        <v>816</v>
+        <v>806</v>
       </c>
       <c r="H609" s="9"/>
       <c r="I609" s="5"/>
@@ -15073,7 +15096,7 @@
         <v>267</v>
       </c>
       <c r="G611" s="33" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="H611" s="9"/>
       <c r="I611" s="5"/>
@@ -15104,7 +15127,7 @@
         <v>280</v>
       </c>
       <c r="G612" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="H612" s="9"/>
       <c r="I612" s="5"/>
@@ -15166,7 +15189,7 @@
         <v>188</v>
       </c>
       <c r="G614" s="33" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="H614" s="9"/>
       <c r="I614" s="5"/>
@@ -15197,7 +15220,7 @@
         <v>189</v>
       </c>
       <c r="G615" s="33" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="H615" s="9"/>
       <c r="I615" s="5"/>
@@ -15290,7 +15313,7 @@
         <v>282</v>
       </c>
       <c r="G618" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="H618" s="9"/>
       <c r="I618" s="5"/>
@@ -15321,7 +15344,7 @@
         <v>191</v>
       </c>
       <c r="G619" s="33" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="H619" s="9"/>
       <c r="I619" s="5"/>
@@ -15716,7 +15739,7 @@
         <v>34</v>
       </c>
       <c r="G634" s="33" t="s">
-        <v>813</v>
+        <v>963</v>
       </c>
       <c r="H634" s="9"/>
       <c r="I634" s="5"/>
@@ -15842,7 +15865,7 @@
         <v>267</v>
       </c>
       <c r="G638" s="33" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="H638" s="9"/>
       <c r="I638" s="5"/>
@@ -15873,7 +15896,7 @@
         <v>280</v>
       </c>
       <c r="G639" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="H639" s="9"/>
       <c r="I639" s="5"/>
@@ -15935,7 +15958,7 @@
         <v>188</v>
       </c>
       <c r="G641" s="33" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="H641" s="9"/>
       <c r="I641" s="5"/>
@@ -15966,7 +15989,7 @@
         <v>189</v>
       </c>
       <c r="G642" s="33" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="H642" s="9"/>
       <c r="I642" s="5"/>
@@ -16059,7 +16082,7 @@
         <v>282</v>
       </c>
       <c r="G645" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="H645" s="9"/>
       <c r="I645" s="5"/>
@@ -16090,7 +16113,7 @@
         <v>191</v>
       </c>
       <c r="G646" s="33" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="H646" s="9"/>
       <c r="I646" s="5"/>
@@ -16485,7 +16508,7 @@
         <v>34</v>
       </c>
       <c r="G661" s="33" t="s">
-        <v>813</v>
+        <v>963</v>
       </c>
       <c r="H661" s="9"/>
       <c r="I661" s="5"/>
@@ -16516,7 +16539,7 @@
         <v>430</v>
       </c>
       <c r="G662" s="20" t="s">
-        <v>815</v>
+        <v>805</v>
       </c>
       <c r="H662" s="9"/>
       <c r="I662" s="5"/>
@@ -16547,7 +16570,7 @@
         <v>430</v>
       </c>
       <c r="G663" s="33" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="H663" s="9"/>
       <c r="I663" s="5"/>
@@ -16611,7 +16634,7 @@
         <v>267</v>
       </c>
       <c r="G665" s="33" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="H665" s="9"/>
       <c r="I665" s="5"/>
@@ -16642,7 +16665,7 @@
         <v>280</v>
       </c>
       <c r="G666" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="H666" s="9"/>
       <c r="I666" s="5"/>
@@ -16704,7 +16727,7 @@
         <v>188</v>
       </c>
       <c r="G668" s="33" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="H668" s="9"/>
       <c r="I668" s="5"/>
@@ -16735,7 +16758,7 @@
         <v>189</v>
       </c>
       <c r="G669" s="33" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="H669" s="9"/>
       <c r="I669" s="5"/>
@@ -16828,7 +16851,7 @@
         <v>282</v>
       </c>
       <c r="G672" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="H672" s="9"/>
       <c r="I672" s="5"/>
@@ -16859,7 +16882,7 @@
         <v>191</v>
       </c>
       <c r="G673" s="33" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="H673" s="9"/>
       <c r="I673" s="5"/>
@@ -17198,7 +17221,7 @@
         <v>429</v>
       </c>
       <c r="B686" s="7" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="C686" s="7"/>
       <c r="D686" s="8"/>
@@ -17221,7 +17244,7 @@
         <v>756</v>
       </c>
       <c r="G687" s="33" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="H687" s="9"/>
       <c r="I687" s="5"/>
@@ -17254,7 +17277,7 @@
         <v>34</v>
       </c>
       <c r="G688" s="20" t="s">
-        <v>798</v>
+        <v>961</v>
       </c>
       <c r="H688" s="9"/>
       <c r="I688" s="5"/>
@@ -17285,7 +17308,7 @@
         <v>430</v>
       </c>
       <c r="G689" s="20" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="H689" s="9"/>
       <c r="I689" s="5"/>
@@ -17316,7 +17339,7 @@
         <v>430</v>
       </c>
       <c r="G690" s="33" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
       <c r="H690" s="9"/>
       <c r="I690" s="5"/>
@@ -17380,7 +17403,7 @@
         <v>267</v>
       </c>
       <c r="G692" s="33" t="s">
-        <v>897</v>
+        <v>887</v>
       </c>
       <c r="H692" s="9"/>
       <c r="I692" s="5"/>
@@ -17411,7 +17434,7 @@
         <v>280</v>
       </c>
       <c r="G693" s="33" t="s">
-        <v>896</v>
+        <v>886</v>
       </c>
       <c r="H693" s="9"/>
       <c r="I693" s="5"/>
@@ -17473,7 +17496,7 @@
         <v>188</v>
       </c>
       <c r="G695" s="20" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="H695" s="9"/>
       <c r="I695" s="5"/>
@@ -17504,7 +17527,7 @@
         <v>189</v>
       </c>
       <c r="G696" s="33" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="H696" s="9"/>
       <c r="I696" s="5"/>
@@ -17597,7 +17620,7 @@
         <v>282</v>
       </c>
       <c r="G699" s="33" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
       <c r="H699" s="9"/>
       <c r="I699" s="5"/>
@@ -17628,7 +17651,7 @@
         <v>191</v>
       </c>
       <c r="G700" s="33" t="s">
-        <v>895</v>
+        <v>885</v>
       </c>
       <c r="H700" s="9"/>
       <c r="I700" s="5"/>
@@ -17967,7 +17990,7 @@
         <v>429</v>
       </c>
       <c r="B713" s="7" t="s">
-        <v>915</v>
+        <v>905</v>
       </c>
       <c r="C713" s="7"/>
       <c r="D713" s="8"/>
@@ -17990,7 +18013,7 @@
         <v>756</v>
       </c>
       <c r="G714" s="33" t="s">
-        <v>935</v>
+        <v>924</v>
       </c>
       <c r="H714" s="9"/>
       <c r="I714" s="5"/>
@@ -18023,7 +18046,7 @@
         <v>34</v>
       </c>
       <c r="G715" s="20" t="s">
-        <v>795</v>
+        <v>958</v>
       </c>
       <c r="H715" s="9"/>
       <c r="I715" s="5"/>
@@ -18054,7 +18077,7 @@
         <v>430</v>
       </c>
       <c r="G716" s="20" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="H716" s="9"/>
       <c r="I716" s="5"/>
@@ -18085,7 +18108,7 @@
         <v>430</v>
       </c>
       <c r="G717" s="33" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="H717" s="9"/>
       <c r="I717" s="5"/>
@@ -18149,7 +18172,7 @@
         <v>267</v>
       </c>
       <c r="G719" s="33" t="s">
-        <v>930</v>
+        <v>919</v>
       </c>
       <c r="H719" s="9"/>
       <c r="I719" s="5"/>
@@ -18180,7 +18203,7 @@
         <v>280</v>
       </c>
       <c r="G720" s="33" t="s">
-        <v>933</v>
+        <v>922</v>
       </c>
       <c r="H720" s="9"/>
       <c r="I720" s="5"/>
@@ -18242,7 +18265,7 @@
         <v>188</v>
       </c>
       <c r="G722" s="20" t="s">
-        <v>931</v>
+        <v>920</v>
       </c>
       <c r="H722" s="9"/>
       <c r="I722" s="5"/>
@@ -18273,7 +18296,7 @@
         <v>189</v>
       </c>
       <c r="G723" s="33" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="H723" s="9"/>
       <c r="I723" s="5"/>
@@ -18366,7 +18389,7 @@
         <v>282</v>
       </c>
       <c r="G726" s="33" t="s">
-        <v>933</v>
+        <v>922</v>
       </c>
       <c r="H726" s="9"/>
       <c r="I726" s="5"/>
@@ -18397,7 +18420,7 @@
         <v>191</v>
       </c>
       <c r="G727" s="33" t="s">
-        <v>930</v>
+        <v>919</v>
       </c>
       <c r="H727" s="9"/>
       <c r="I727" s="5"/>
@@ -18736,7 +18759,7 @@
         <v>429</v>
       </c>
       <c r="B740" s="7" t="s">
-        <v>916</v>
+        <v>906</v>
       </c>
       <c r="C740" s="7"/>
       <c r="D740" s="8"/>
@@ -18759,7 +18782,7 @@
         <v>756</v>
       </c>
       <c r="G741" s="33" t="s">
-        <v>934</v>
+        <v>923</v>
       </c>
       <c r="H741" s="9"/>
       <c r="I741" s="5"/>
@@ -18792,7 +18815,7 @@
         <v>34</v>
       </c>
       <c r="G742" s="20" t="s">
-        <v>795</v>
+        <v>958</v>
       </c>
       <c r="H742" s="9"/>
       <c r="I742" s="5"/>
@@ -18823,7 +18846,7 @@
         <v>430</v>
       </c>
       <c r="G743" s="20" t="s">
-        <v>918</v>
+        <v>908</v>
       </c>
       <c r="H743" s="9"/>
       <c r="I743" s="5"/>
@@ -18854,7 +18877,7 @@
         <v>430</v>
       </c>
       <c r="G744" s="33" t="s">
-        <v>918</v>
+        <v>908</v>
       </c>
       <c r="H744" s="9"/>
       <c r="I744" s="5"/>
@@ -18918,7 +18941,7 @@
         <v>267</v>
       </c>
       <c r="G746" s="33" t="s">
-        <v>929</v>
+        <v>918</v>
       </c>
       <c r="H746" s="9"/>
       <c r="I746" s="5"/>
@@ -18949,7 +18972,7 @@
         <v>280</v>
       </c>
       <c r="G747" s="33" t="s">
-        <v>933</v>
+        <v>922</v>
       </c>
       <c r="H747" s="9"/>
       <c r="I747" s="5"/>
@@ -19011,7 +19034,7 @@
         <v>188</v>
       </c>
       <c r="G749" s="20" t="s">
-        <v>932</v>
+        <v>921</v>
       </c>
       <c r="H749" s="9"/>
       <c r="I749" s="5"/>
@@ -19042,7 +19065,7 @@
         <v>189</v>
       </c>
       <c r="G750" s="33" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="H750" s="9"/>
       <c r="I750" s="5"/>
@@ -19135,7 +19158,7 @@
         <v>282</v>
       </c>
       <c r="G753" s="33" t="s">
-        <v>933</v>
+        <v>922</v>
       </c>
       <c r="H753" s="9"/>
       <c r="I753" s="5"/>
@@ -19166,7 +19189,7 @@
         <v>191</v>
       </c>
       <c r="G754" s="33" t="s">
-        <v>929</v>
+        <v>918</v>
       </c>
       <c r="H754" s="9"/>
       <c r="I754" s="5"/>
@@ -19505,7 +19528,7 @@
         <v>429</v>
       </c>
       <c r="B767" s="7" t="s">
-        <v>937</v>
+        <v>926</v>
       </c>
       <c r="C767" s="7"/>
       <c r="D767" s="8"/>
@@ -19515,7 +19538,7 @@
       <c r="H767" s="50"/>
     </row>
     <row r="768" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A768" s="23" t="s">
+      <c r="A768" s="19" t="s">
         <v>348</v>
       </c>
       <c r="B768" s="10" t="s">
@@ -19528,7 +19551,7 @@
         <v>756</v>
       </c>
       <c r="G768" s="20" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="I768" s="5"/>
       <c r="J768" s="5"/>
@@ -19547,7 +19570,7 @@
       <c r="W768" s="5"/>
     </row>
     <row r="769" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A769" s="23" t="s">
+      <c r="A769" s="19" t="s">
         <v>330</v>
       </c>
       <c r="B769" s="10" t="s">
@@ -19560,7 +19583,7 @@
         <v>34</v>
       </c>
       <c r="G769" s="20" t="s">
-        <v>799</v>
+        <v>962</v>
       </c>
       <c r="I769" s="5"/>
       <c r="J769" s="5"/>
@@ -19579,7 +19602,7 @@
       <c r="W769" s="5"/>
     </row>
     <row r="770" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A770" s="23" t="s">
+      <c r="A770" s="19" t="s">
         <v>349</v>
       </c>
       <c r="B770" s="10"/>
@@ -19590,7 +19613,7 @@
         <v>430</v>
       </c>
       <c r="G770" s="20" t="s">
-        <v>938</v>
+        <v>927</v>
       </c>
       <c r="H770" s="20"/>
       <c r="I770" s="5"/>
@@ -19610,7 +19633,7 @@
       <c r="W770" s="5"/>
     </row>
     <row r="771" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A771" s="23" t="s">
+      <c r="A771" s="19" t="s">
         <v>350</v>
       </c>
       <c r="B771" s="10"/>
@@ -19621,7 +19644,7 @@
         <v>430</v>
       </c>
       <c r="G771" s="33" t="s">
-        <v>938</v>
+        <v>927</v>
       </c>
       <c r="H771" s="33"/>
       <c r="I771" s="5"/>
@@ -19641,7 +19664,7 @@
       <c r="W771" s="5"/>
     </row>
     <row r="772" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A772" s="23" t="s">
+      <c r="A772" s="19" t="s">
         <v>351</v>
       </c>
       <c r="B772" s="10"/>
@@ -19671,7 +19694,7 @@
       <c r="W772" s="5"/>
     </row>
     <row r="773" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A773" s="23" t="s">
+      <c r="A773" s="19" t="s">
         <v>352</v>
       </c>
       <c r="B773" s="10" t="s">
@@ -19703,7 +19726,7 @@
       <c r="W773" s="5"/>
     </row>
     <row r="774" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A774" s="23" t="s">
+      <c r="A774" s="19" t="s">
         <v>332</v>
       </c>
       <c r="B774" s="10"/>
@@ -19733,7 +19756,7 @@
       <c r="W774" s="5"/>
     </row>
     <row r="775" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A775" s="23" t="s">
+      <c r="A775" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B775" s="10"/>
@@ -19763,7 +19786,7 @@
       <c r="W775" s="5"/>
     </row>
     <row r="776" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A776" s="23" t="s">
+      <c r="A776" s="19" t="s">
         <v>354</v>
       </c>
       <c r="B776" s="10"/>
@@ -19793,7 +19816,7 @@
       <c r="W776" s="5"/>
     </row>
     <row r="777" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A777" s="23" t="s">
+      <c r="A777" s="19" t="s">
         <v>353</v>
       </c>
       <c r="B777" s="10"/>
@@ -19804,7 +19827,7 @@
         <v>189</v>
       </c>
       <c r="G777" s="20" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="I777" s="5"/>
       <c r="J777" s="5"/>
@@ -19823,7 +19846,7 @@
       <c r="W777" s="5"/>
     </row>
     <row r="778" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A778" s="23" t="s">
+      <c r="A778" s="19" t="s">
         <v>355</v>
       </c>
       <c r="B778" s="10"/>
@@ -19853,7 +19876,7 @@
       <c r="W778" s="5"/>
     </row>
     <row r="779" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A779" s="23" t="s">
+      <c r="A779" s="19" t="s">
         <v>341</v>
       </c>
       <c r="B779" s="10"/>
@@ -19883,7 +19906,7 @@
       <c r="W779" s="5"/>
     </row>
     <row r="780" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A780" s="23" t="s">
+      <c r="A780" s="19" t="s">
         <v>356</v>
       </c>
       <c r="B780" s="10"/>
@@ -19913,7 +19936,7 @@
       <c r="W780" s="5"/>
     </row>
     <row r="781" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A781" s="23" t="s">
+      <c r="A781" s="19" t="s">
         <v>357</v>
       </c>
       <c r="B781" s="10"/>
@@ -19943,7 +19966,7 @@
       <c r="W781" s="5"/>
     </row>
     <row r="782" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A782" s="23" t="s">
+      <c r="A782" s="19" t="s">
         <v>359</v>
       </c>
       <c r="B782" s="10"/>
@@ -19973,7 +19996,7 @@
       <c r="W782" s="5"/>
     </row>
     <row r="783" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A783" s="23" t="s">
+      <c r="A783" s="19" t="s">
         <v>360</v>
       </c>
       <c r="B783" s="10"/>
@@ -20003,7 +20026,7 @@
       <c r="W783" s="5"/>
     </row>
     <row r="784" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A784" s="23" t="s">
+      <c r="A784" s="19" t="s">
         <v>361</v>
       </c>
       <c r="B784" s="10"/>
@@ -20033,7 +20056,7 @@
       <c r="W784" s="5"/>
     </row>
     <row r="785" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A785" s="23" t="s">
+      <c r="A785" s="19" t="s">
         <v>362</v>
       </c>
       <c r="B785" s="10"/>
@@ -20063,7 +20086,7 @@
       <c r="W785" s="5"/>
     </row>
     <row r="786" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A786" s="23" t="s">
+      <c r="A786" s="19" t="s">
         <v>363</v>
       </c>
       <c r="B786" s="10"/>
@@ -20093,7 +20116,7 @@
       <c r="W786" s="5"/>
     </row>
     <row r="787" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A787" s="23" t="s">
+      <c r="A787" s="19" t="s">
         <v>364</v>
       </c>
       <c r="B787" s="10"/>
@@ -20123,7 +20146,7 @@
       <c r="W787" s="5"/>
     </row>
     <row r="788" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A788" s="23" t="s">
+      <c r="A788" s="19" t="s">
         <v>618</v>
       </c>
       <c r="B788" s="10"/>
@@ -20153,7 +20176,7 @@
       <c r="W788" s="5"/>
     </row>
     <row r="789" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A789" s="23" t="s">
+      <c r="A789" s="19" t="s">
         <v>638</v>
       </c>
       <c r="B789" s="10"/>
@@ -20168,7 +20191,7 @@
       </c>
     </row>
     <row r="790" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A790" s="23" t="s">
+      <c r="A790" s="19" t="s">
         <v>639</v>
       </c>
       <c r="B790" s="10"/>
@@ -20183,7 +20206,7 @@
       </c>
     </row>
     <row r="791" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A791" s="23" t="s">
+      <c r="A791" s="19" t="s">
         <v>640</v>
       </c>
       <c r="B791" s="10"/>
@@ -20198,7 +20221,7 @@
       </c>
     </row>
     <row r="792" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A792" s="23" t="s">
+      <c r="A792" s="19" t="s">
         <v>641</v>
       </c>
       <c r="B792" s="10"/>
@@ -20213,7 +20236,7 @@
       </c>
     </row>
     <row r="793" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A793" s="23" t="s">
+      <c r="A793" s="19" t="s">
         <v>735</v>
       </c>
       <c r="B793" s="10"/>
@@ -20250,7 +20273,7 @@
         <v>429</v>
       </c>
       <c r="B794" s="7" t="s">
-        <v>911</v>
+        <v>901</v>
       </c>
       <c r="C794" s="7"/>
       <c r="D794" s="8"/>
@@ -20273,7 +20296,7 @@
         <v>756</v>
       </c>
       <c r="G795" s="33" t="s">
-        <v>942</v>
+        <v>931</v>
       </c>
       <c r="H795" s="9"/>
       <c r="I795" s="5"/>
@@ -20306,7 +20329,7 @@
         <v>34</v>
       </c>
       <c r="G796" s="20" t="s">
-        <v>799</v>
+        <v>962</v>
       </c>
       <c r="H796" s="9"/>
       <c r="I796" s="5"/>
@@ -20337,7 +20360,7 @@
         <v>430</v>
       </c>
       <c r="G797" s="20" t="s">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="H797" s="9"/>
       <c r="I797" s="5"/>
@@ -20368,7 +20391,7 @@
         <v>430</v>
       </c>
       <c r="G798" s="33" t="s">
-        <v>952</v>
+        <v>940</v>
       </c>
       <c r="H798" s="9"/>
       <c r="I798" s="5"/>
@@ -20432,7 +20455,7 @@
         <v>267</v>
       </c>
       <c r="G800" s="33" t="s">
-        <v>944</v>
+        <v>933</v>
       </c>
       <c r="H800" s="9"/>
       <c r="I800" s="5"/>
@@ -20463,7 +20486,7 @@
         <v>280</v>
       </c>
       <c r="G801" s="33" t="s">
-        <v>943</v>
+        <v>932</v>
       </c>
       <c r="H801" s="9"/>
       <c r="I801" s="5"/>
@@ -20525,7 +20548,7 @@
         <v>188</v>
       </c>
       <c r="G803" s="20" t="s">
-        <v>953</v>
+        <v>941</v>
       </c>
       <c r="H803" s="9"/>
       <c r="I803" s="5"/>
@@ -20649,7 +20672,7 @@
         <v>282</v>
       </c>
       <c r="G807" s="33" t="s">
-        <v>943</v>
+        <v>932</v>
       </c>
       <c r="H807" s="9"/>
       <c r="I807" s="5"/>
@@ -20680,7 +20703,7 @@
         <v>191</v>
       </c>
       <c r="G808" s="33" t="s">
-        <v>944</v>
+        <v>933</v>
       </c>
       <c r="H808" s="9"/>
       <c r="I808" s="5"/>
@@ -21019,7 +21042,7 @@
         <v>429</v>
       </c>
       <c r="B821" s="7" t="s">
-        <v>945</v>
+        <v>934</v>
       </c>
       <c r="C821" s="7"/>
       <c r="D821" s="8"/>
@@ -21042,7 +21065,7 @@
         <v>756</v>
       </c>
       <c r="G822" s="20" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="H822" s="9"/>
       <c r="I822" s="5"/>
@@ -21075,7 +21098,7 @@
         <v>34</v>
       </c>
       <c r="G823" s="20" t="s">
-        <v>799</v>
+        <v>962</v>
       </c>
       <c r="H823" s="9"/>
       <c r="I823" s="5"/>
@@ -21106,7 +21129,7 @@
         <v>430</v>
       </c>
       <c r="G824" s="20" t="s">
-        <v>815</v>
+        <v>805</v>
       </c>
       <c r="H824" s="9"/>
       <c r="I824" s="5"/>
@@ -21136,7 +21159,9 @@
       <c r="F825" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="G825" s="55"/>
+      <c r="G825" s="20" t="s">
+        <v>807</v>
+      </c>
       <c r="H825" s="9"/>
       <c r="I825" s="5"/>
       <c r="J825" s="5"/>
@@ -21477,8 +21502,8 @@
       <c r="F836" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="G836" s="55" t="s">
-        <v>20</v>
+      <c r="G836" s="20" t="b">
+        <v>1</v>
       </c>
       <c r="H836" s="9"/>
       <c r="I836" s="5"/>
@@ -21846,7 +21871,7 @@
         <v>429</v>
       </c>
       <c r="B848" s="7" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C848" s="7"/>
       <c r="D848" s="8"/>
@@ -21869,7 +21894,7 @@
         <v>756</v>
       </c>
       <c r="G849" s="33" t="s">
-        <v>948</v>
+        <v>936</v>
       </c>
       <c r="H849" s="9"/>
       <c r="I849" s="5"/>
@@ -21902,7 +21927,7 @@
         <v>34</v>
       </c>
       <c r="G850" s="20" t="s">
-        <v>795</v>
+        <v>958</v>
       </c>
       <c r="H850" s="9"/>
       <c r="I850" s="5"/>
@@ -21933,7 +21958,7 @@
         <v>430</v>
       </c>
       <c r="G851" s="20" t="s">
-        <v>949</v>
+        <v>937</v>
       </c>
       <c r="H851" s="9"/>
       <c r="I851" s="5"/>
@@ -21964,7 +21989,7 @@
         <v>430</v>
       </c>
       <c r="G852" s="33" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="H852" s="9"/>
       <c r="I852" s="5"/>
@@ -22027,8 +22052,8 @@
       <c r="F854" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="G854" s="54" t="s">
-        <v>180</v>
+      <c r="G854" s="33" t="s">
+        <v>946</v>
       </c>
       <c r="H854" s="9"/>
       <c r="I854" s="5"/>
@@ -22058,8 +22083,8 @@
       <c r="F855" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="G855" s="54" t="s">
-        <v>180</v>
+      <c r="G855" s="33" t="s">
+        <v>949</v>
       </c>
       <c r="H855" s="9"/>
       <c r="I855" s="5"/>
@@ -22120,7 +22145,9 @@
       <c r="F857" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="G857" s="55"/>
+      <c r="G857" s="20" t="s">
+        <v>950</v>
+      </c>
       <c r="H857" s="9"/>
       <c r="I857" s="5"/>
       <c r="J857" s="5"/>
@@ -22149,8 +22176,8 @@
       <c r="F858" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="G858" s="54" t="s">
-        <v>180</v>
+      <c r="G858" s="33" t="s">
+        <v>947</v>
       </c>
       <c r="H858" s="9"/>
       <c r="I858" s="5"/>
@@ -22242,8 +22269,8 @@
       <c r="F861" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="G861" s="54" t="s">
-        <v>180</v>
+      <c r="G861" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H861" s="9"/>
       <c r="I861" s="5"/>
@@ -22273,8 +22300,8 @@
       <c r="F862" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="G862" s="54" t="s">
-        <v>180</v>
+      <c r="G862" s="33" t="s">
+        <v>946</v>
       </c>
       <c r="H862" s="9"/>
       <c r="I862" s="5"/>
@@ -22304,8 +22331,8 @@
       <c r="F863" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="G863" s="54" t="s">
-        <v>180</v>
+      <c r="G863" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H863" s="9"/>
       <c r="I863" s="5"/>
@@ -22335,8 +22362,8 @@
       <c r="F864" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="G864" s="54" t="s">
-        <v>180</v>
+      <c r="G864" s="33" t="s">
+        <v>303</v>
       </c>
       <c r="H864" s="9"/>
       <c r="I864" s="5"/>
@@ -22366,8 +22393,8 @@
       <c r="F865" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G865" s="54" t="s">
-        <v>180</v>
+      <c r="G865" s="33" t="b">
+        <v>1</v>
       </c>
       <c r="H865" s="9"/>
       <c r="I865" s="5"/>
@@ -22397,7 +22424,9 @@
       <c r="F866" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="G866" s="55"/>
+      <c r="G866" s="20" t="s">
+        <v>951</v>
+      </c>
       <c r="H866" s="9"/>
       <c r="I866" s="5"/>
       <c r="J866" s="5"/>
@@ -22426,7 +22455,9 @@
       <c r="F867" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G867" s="55"/>
+      <c r="G867" s="20" t="s">
+        <v>952</v>
+      </c>
       <c r="H867" s="9"/>
       <c r="I867" s="5"/>
       <c r="J867" s="5"/>
@@ -22456,7 +22487,7 @@
         <v>198</v>
       </c>
       <c r="G868" s="54" t="s">
-        <v>180</v>
+        <v>964</v>
       </c>
       <c r="H868" s="9"/>
       <c r="I868" s="5"/>
@@ -22487,7 +22518,7 @@
         <v>619</v>
       </c>
       <c r="G869" s="54" t="s">
-        <v>180</v>
+        <v>965</v>
       </c>
       <c r="H869" s="9"/>
       <c r="I869" s="5"/>
@@ -22517,8 +22548,8 @@
       <c r="F870" s="6" t="s">
         <v>642</v>
       </c>
-      <c r="G870" s="54" t="s">
-        <v>180</v>
+      <c r="G870" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H870" s="9"/>
     </row>
@@ -22533,8 +22564,8 @@
       <c r="F871" s="6" t="s">
         <v>643</v>
       </c>
-      <c r="G871" s="54" t="s">
-        <v>180</v>
+      <c r="G871" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H871" s="9"/>
     </row>
@@ -22549,8 +22580,8 @@
       <c r="F872" s="6" t="s">
         <v>644</v>
       </c>
-      <c r="G872" s="54" t="s">
-        <v>180</v>
+      <c r="G872" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H872" s="9"/>
     </row>
@@ -22565,8 +22596,8 @@
       <c r="F873" s="6" t="s">
         <v>645</v>
       </c>
-      <c r="G873" s="54" t="s">
-        <v>180</v>
+      <c r="G873" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H873" s="9"/>
     </row>
@@ -22584,8 +22615,8 @@
       <c r="F874" s="6" t="s">
         <v>736</v>
       </c>
-      <c r="G874" s="54" t="s">
-        <v>180</v>
+      <c r="G874" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H874" s="9"/>
       <c r="I874" s="5"/>
@@ -22609,7 +22640,7 @@
         <v>429</v>
       </c>
       <c r="B875" s="7" t="s">
-        <v>957</v>
+        <v>945</v>
       </c>
       <c r="C875" s="7"/>
       <c r="D875" s="8"/>
@@ -22619,7 +22650,7 @@
       <c r="H875" s="50"/>
     </row>
     <row r="876" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A876" s="23" t="s">
+      <c r="A876" s="19" t="s">
         <v>348</v>
       </c>
       <c r="B876" s="10" t="s">
@@ -22652,7 +22683,7 @@
       <c r="W876" s="5"/>
     </row>
     <row r="877" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A877" s="23" t="s">
+      <c r="A877" s="19" t="s">
         <v>330</v>
       </c>
       <c r="B877" s="10" t="s">
@@ -22665,7 +22696,7 @@
         <v>34</v>
       </c>
       <c r="G877" s="33" t="s">
-        <v>813</v>
+        <v>963</v>
       </c>
       <c r="H877" s="9"/>
       <c r="I877" s="5"/>
@@ -22685,7 +22716,7 @@
       <c r="W877" s="5"/>
     </row>
     <row r="878" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A878" s="23" t="s">
+      <c r="A878" s="19" t="s">
         <v>349</v>
       </c>
       <c r="B878" s="10"/>
@@ -22696,7 +22727,7 @@
         <v>430</v>
       </c>
       <c r="G878" s="20" t="s">
-        <v>938</v>
+        <v>927</v>
       </c>
       <c r="H878" s="9"/>
       <c r="I878" s="5"/>
@@ -22716,7 +22747,7 @@
       <c r="W878" s="5"/>
     </row>
     <row r="879" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A879" s="23" t="s">
+      <c r="A879" s="19" t="s">
         <v>350</v>
       </c>
       <c r="B879" s="10"/>
@@ -22727,7 +22758,7 @@
         <v>430</v>
       </c>
       <c r="G879" s="20" t="s">
-        <v>938</v>
+        <v>927</v>
       </c>
       <c r="H879" s="9"/>
       <c r="I879" s="5"/>
@@ -22747,7 +22778,7 @@
       <c r="W879" s="5"/>
     </row>
     <row r="880" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A880" s="23" t="s">
+      <c r="A880" s="19" t="s">
         <v>351</v>
       </c>
       <c r="B880" s="10"/>
@@ -22778,7 +22809,7 @@
       <c r="W880" s="5"/>
     </row>
     <row r="881" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A881" s="23" t="s">
+      <c r="A881" s="19" t="s">
         <v>352</v>
       </c>
       <c r="B881" s="10" t="s">
@@ -22791,7 +22822,7 @@
         <v>267</v>
       </c>
       <c r="G881" s="33" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="H881" s="9"/>
       <c r="I881" s="5"/>
@@ -22811,7 +22842,7 @@
       <c r="W881" s="5"/>
     </row>
     <row r="882" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A882" s="23" t="s">
+      <c r="A882" s="19" t="s">
         <v>332</v>
       </c>
       <c r="B882" s="10"/>
@@ -22822,7 +22853,7 @@
         <v>280</v>
       </c>
       <c r="G882" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="H882" s="9"/>
       <c r="I882" s="5"/>
@@ -22842,7 +22873,7 @@
       <c r="W882" s="5"/>
     </row>
     <row r="883" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A883" s="23" t="s">
+      <c r="A883" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B883" s="10"/>
@@ -22873,7 +22904,7 @@
       <c r="W883" s="5"/>
     </row>
     <row r="884" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A884" s="23" t="s">
+      <c r="A884" s="19" t="s">
         <v>354</v>
       </c>
       <c r="B884" s="10"/>
@@ -22884,7 +22915,7 @@
         <v>188</v>
       </c>
       <c r="G884" s="33" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="H884" s="9"/>
       <c r="I884" s="5"/>
@@ -22904,7 +22935,7 @@
       <c r="W884" s="5"/>
     </row>
     <row r="885" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A885" s="23" t="s">
+      <c r="A885" s="19" t="s">
         <v>353</v>
       </c>
       <c r="B885" s="10"/>
@@ -22915,7 +22946,7 @@
         <v>189</v>
       </c>
       <c r="G885" s="33" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="H885" s="9"/>
       <c r="I885" s="5"/>
@@ -22935,7 +22966,7 @@
       <c r="W885" s="5"/>
     </row>
     <row r="886" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A886" s="23" t="s">
+      <c r="A886" s="19" t="s">
         <v>355</v>
       </c>
       <c r="B886" s="10"/>
@@ -22966,7 +22997,7 @@
       <c r="W886" s="5"/>
     </row>
     <row r="887" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A887" s="23" t="s">
+      <c r="A887" s="19" t="s">
         <v>341</v>
       </c>
       <c r="B887" s="10"/>
@@ -22997,7 +23028,7 @@
       <c r="W887" s="5"/>
     </row>
     <row r="888" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A888" s="23" t="s">
+      <c r="A888" s="19" t="s">
         <v>356</v>
       </c>
       <c r="B888" s="10"/>
@@ -23008,7 +23039,7 @@
         <v>282</v>
       </c>
       <c r="G888" s="33" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="H888" s="9"/>
       <c r="I888" s="5"/>
@@ -23028,7 +23059,7 @@
       <c r="W888" s="5"/>
     </row>
     <row r="889" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A889" s="23" t="s">
+      <c r="A889" s="19" t="s">
         <v>357</v>
       </c>
       <c r="B889" s="10"/>
@@ -23039,7 +23070,7 @@
         <v>191</v>
       </c>
       <c r="G889" s="33" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="H889" s="9"/>
       <c r="I889" s="5"/>
@@ -23059,7 +23090,7 @@
       <c r="W889" s="5"/>
     </row>
     <row r="890" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A890" s="23" t="s">
+      <c r="A890" s="19" t="s">
         <v>359</v>
       </c>
       <c r="B890" s="10"/>
@@ -23090,7 +23121,7 @@
       <c r="W890" s="5"/>
     </row>
     <row r="891" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A891" s="23" t="s">
+      <c r="A891" s="19" t="s">
         <v>360</v>
       </c>
       <c r="B891" s="10"/>
@@ -23121,7 +23152,7 @@
       <c r="W891" s="5"/>
     </row>
     <row r="892" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A892" s="23" t="s">
+      <c r="A892" s="19" t="s">
         <v>361</v>
       </c>
       <c r="B892" s="10"/>
@@ -23152,7 +23183,7 @@
       <c r="W892" s="5"/>
     </row>
     <row r="893" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A893" s="23" t="s">
+      <c r="A893" s="19" t="s">
         <v>362</v>
       </c>
       <c r="B893" s="10"/>
@@ -23183,7 +23214,7 @@
       <c r="W893" s="5"/>
     </row>
     <row r="894" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A894" s="23" t="s">
+      <c r="A894" s="19" t="s">
         <v>363</v>
       </c>
       <c r="B894" s="10"/>
@@ -23214,7 +23245,7 @@
       <c r="W894" s="5"/>
     </row>
     <row r="895" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A895" s="23" t="s">
+      <c r="A895" s="19" t="s">
         <v>364</v>
       </c>
       <c r="B895" s="10"/>
@@ -23245,7 +23276,7 @@
       <c r="W895" s="5"/>
     </row>
     <row r="896" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A896" s="23" t="s">
+      <c r="A896" s="19" t="s">
         <v>618</v>
       </c>
       <c r="B896" s="10"/>
@@ -23276,7 +23307,7 @@
       <c r="W896" s="5"/>
     </row>
     <row r="897" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A897" s="23" t="s">
+      <c r="A897" s="19" t="s">
         <v>638</v>
       </c>
       <c r="B897" s="10"/>
@@ -23292,7 +23323,7 @@
       <c r="H897" s="9"/>
     </row>
     <row r="898" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A898" s="23" t="s">
+      <c r="A898" s="19" t="s">
         <v>639</v>
       </c>
       <c r="B898" s="10"/>
@@ -23308,7 +23339,7 @@
       <c r="H898" s="9"/>
     </row>
     <row r="899" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A899" s="23" t="s">
+      <c r="A899" s="19" t="s">
         <v>640</v>
       </c>
       <c r="B899" s="10"/>
@@ -23324,7 +23355,7 @@
       <c r="H899" s="9"/>
     </row>
     <row r="900" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A900" s="23" t="s">
+      <c r="A900" s="19" t="s">
         <v>641</v>
       </c>
       <c r="B900" s="10"/>
@@ -23340,7 +23371,7 @@
       <c r="H900" s="9"/>
     </row>
     <row r="901" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A901" s="23" t="s">
+      <c r="A901" s="19" t="s">
         <v>735</v>
       </c>
       <c r="B901" s="10"/>
@@ -24134,7 +24165,7 @@
   <customSheetViews>
     <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{48AEEF92-483D-4AA4-9D0E-8401182909DF}">
+      <autoFilter ref="A2:N83" xr:uid="{FA8F74EB-A80F-4ECB-A4CB-C49D3A02BDFE}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="-"/>
@@ -24145,7 +24176,7 @@
     </customSheetView>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{21E430C1-848D-419F-94D5-2DEE508A6173}">
+      <autoFilter ref="A1:AB1210" xr:uid="{B0595F93-F55B-4BFA-82C5-5B0656AC916A}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
@@ -24290,7 +24321,7 @@
         <v>174</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>828</v>
+        <v>818</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -24324,7 +24355,7 @@
         <v>175</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>828</v>
+        <v>818</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -24385,7 +24416,7 @@
         <v>146</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -24486,7 +24517,7 @@
         <v>144</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>829</v>
+        <v>819</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -24550,7 +24581,7 @@
         <v>143</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>828</v>
+        <v>818</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>180</v>
@@ -24576,7 +24607,7 @@
         <v>677</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>826</v>
+        <v>816</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
@@ -24605,7 +24636,7 @@
         <v>589</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="H14" s="6"/>
     </row>
@@ -24626,10 +24657,10 @@
         <v>50</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>926</v>
+        <v>915</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>828</v>
+        <v>818</v>
       </c>
       <c r="H15" s="6"/>
     </row>
@@ -24653,7 +24684,7 @@
         <v>278</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>864</v>
+        <v>854</v>
       </c>
       <c r="H16" s="6"/>
     </row>
@@ -24675,7 +24706,7 @@
         <v>99</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
       <c r="H17" s="6"/>
     </row>
@@ -24693,7 +24724,7 @@
         <v>35</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>830</v>
+        <v>820</v>
       </c>
       <c r="H18" s="6"/>
     </row>
@@ -24711,7 +24742,7 @@
         <v>100</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>831</v>
+        <v>821</v>
       </c>
       <c r="H19" s="6"/>
     </row>
@@ -24733,7 +24764,7 @@
         <v>279</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>954</v>
+        <v>942</v>
       </c>
       <c r="H20" s="6"/>
     </row>
@@ -24770,10 +24801,10 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c r="H22" s="6"/>
     </row>
@@ -24788,7 +24819,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>20</v>
@@ -24809,7 +24840,7 @@
         <v>40</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>833</v>
+        <v>823</v>
       </c>
       <c r="H24" s="6"/>
     </row>
@@ -24824,10 +24855,10 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>927</v>
+        <v>916</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>906</v>
+        <v>896</v>
       </c>
       <c r="H25" s="41"/>
     </row>
@@ -24863,7 +24894,7 @@
         <v>36</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="H27" s="6"/>
     </row>
@@ -25013,7 +25044,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="45" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="27" t="s">
@@ -25022,16 +25053,16 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="G36" s="41" t="s">
-        <v>939</v>
+        <v>928</v>
       </c>
       <c r="H36" s="41"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="45" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="27" t="s">
@@ -25040,10 +25071,10 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="G37" s="41" t="s">
-        <v>940</v>
+        <v>929</v>
       </c>
       <c r="H37" s="41"/>
     </row>
@@ -25058,10 +25089,10 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>941</v>
+        <v>930</v>
       </c>
       <c r="H38" s="41"/>
     </row>
@@ -25070,7 +25101,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
@@ -25099,7 +25130,7 @@
         <v>680</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="4"/>
@@ -25122,7 +25153,7 @@
         <v>44</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="4"/>
@@ -25145,7 +25176,7 @@
         <v>101</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="4"/>
@@ -25164,7 +25195,7 @@
         <v>102</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>846</v>
+        <v>836</v>
       </c>
       <c r="I43" s="28" t="s">
         <v>180</v>
@@ -25184,7 +25215,7 @@
         <v>103</v>
       </c>
       <c r="G44" s="41" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="4"/>
@@ -25203,7 +25234,7 @@
         <v>45</v>
       </c>
       <c r="G45" s="41" t="s">
-        <v>842</v>
+        <v>832</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="4"/>
@@ -25222,7 +25253,7 @@
         <v>46</v>
       </c>
       <c r="G46" s="41" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="4"/>
@@ -25241,7 +25272,7 @@
         <v>47</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="4"/>
@@ -25296,7 +25327,7 @@
         <v>148</v>
       </c>
       <c r="G50" s="41" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="4"/>
@@ -25315,7 +25346,7 @@
         <v>14</v>
       </c>
       <c r="G51" s="41" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="4"/>
@@ -25334,7 +25365,7 @@
         <v>50</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="4"/>
@@ -25406,7 +25437,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>20</v>
@@ -25465,7 +25496,7 @@
         <v>55</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>854</v>
+        <v>844</v>
       </c>
       <c r="I59" s="4"/>
     </row>
@@ -25556,7 +25587,7 @@
         <v>59</v>
       </c>
       <c r="G64" s="41" t="s">
-        <v>851</v>
+        <v>841</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="4"/>
@@ -25575,7 +25606,7 @@
         <v>60</v>
       </c>
       <c r="G65" s="41" t="s">
-        <v>852</v>
+        <v>842</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="4"/>
@@ -25594,7 +25625,7 @@
         <v>61</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>853</v>
+        <v>843</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="4"/>
@@ -25613,7 +25644,7 @@
         <v>575</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="4"/>
@@ -25632,7 +25663,7 @@
         <v>427</v>
       </c>
       <c r="G68" s="41" t="s">
-        <v>859</v>
+        <v>849</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="4"/>
@@ -25651,7 +25682,7 @@
         <v>62</v>
       </c>
       <c r="G69" s="41" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="4"/>
@@ -25742,7 +25773,7 @@
         <v>67</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>871</v>
+        <v>861</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="4"/>
@@ -25761,7 +25792,7 @@
         <v>535</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>872</v>
+        <v>862</v>
       </c>
       <c r="H75" s="6"/>
       <c r="I75" s="4"/>
@@ -25836,7 +25867,7 @@
         <v>590</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>855</v>
+        <v>845</v>
       </c>
       <c r="I79" s="28" t="s">
         <v>180</v>
@@ -25856,7 +25887,7 @@
         <v>650</v>
       </c>
       <c r="G80" s="41" t="s">
-        <v>850</v>
+        <v>840</v>
       </c>
       <c r="H80" s="41"/>
       <c r="I80" s="4"/>
@@ -25940,7 +25971,7 @@
         <v>42</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="8"/>
@@ -25969,7 +26000,7 @@
         <v>680</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>857</v>
+        <v>847</v>
       </c>
       <c r="H86" s="6"/>
     </row>
@@ -25991,7 +26022,7 @@
         <v>44</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="H87" s="6"/>
     </row>
@@ -26013,7 +26044,7 @@
         <v>101</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="H88" s="6"/>
     </row>
@@ -26031,7 +26062,7 @@
         <v>102</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>846</v>
+        <v>836</v>
       </c>
       <c r="H89" s="6"/>
     </row>
@@ -26049,7 +26080,7 @@
         <v>103</v>
       </c>
       <c r="G90" s="41" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
       <c r="H90" s="6"/>
     </row>
@@ -26067,7 +26098,7 @@
         <v>45</v>
       </c>
       <c r="G91" s="41" t="s">
-        <v>842</v>
+        <v>832</v>
       </c>
       <c r="H91" s="6"/>
     </row>
@@ -26085,7 +26116,7 @@
         <v>46</v>
       </c>
       <c r="G92" s="41" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="H92" s="6"/>
     </row>
@@ -26103,7 +26134,7 @@
         <v>47</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="H93" s="6"/>
     </row>
@@ -26157,7 +26188,7 @@
         <v>148</v>
       </c>
       <c r="G96" s="41" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="H96" s="6"/>
     </row>
@@ -26175,7 +26206,7 @@
         <v>14</v>
       </c>
       <c r="G97" s="41" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="H97" s="6"/>
     </row>
@@ -26193,7 +26224,7 @@
         <v>50</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="H98" s="6"/>
     </row>
@@ -26264,10 +26295,10 @@
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
       <c r="F102" s="6" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="G102" s="41" t="s">
-        <v>858</v>
+        <v>848</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -26320,7 +26351,7 @@
         <v>55</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>854</v>
+        <v>844</v>
       </c>
       <c r="H105" s="6"/>
     </row>
@@ -26410,7 +26441,7 @@
         <v>59</v>
       </c>
       <c r="G110" s="41" t="s">
-        <v>851</v>
+        <v>841</v>
       </c>
       <c r="H110" s="6"/>
     </row>
@@ -26428,7 +26459,7 @@
         <v>60</v>
       </c>
       <c r="G111" s="41" t="s">
-        <v>852</v>
+        <v>842</v>
       </c>
       <c r="H111" s="6"/>
     </row>
@@ -26446,7 +26477,7 @@
         <v>61</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>853</v>
+        <v>843</v>
       </c>
       <c r="H112" s="6"/>
     </row>
@@ -26464,7 +26495,7 @@
         <v>575</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>857</v>
+        <v>847</v>
       </c>
       <c r="H113" s="6"/>
     </row>
@@ -26482,7 +26513,7 @@
         <v>427</v>
       </c>
       <c r="G114" s="41" t="s">
-        <v>859</v>
+        <v>849</v>
       </c>
       <c r="H114" s="6"/>
     </row>
@@ -26500,7 +26531,7 @@
         <v>62</v>
       </c>
       <c r="G115" s="41" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="H115" s="6"/>
     </row>
@@ -26590,7 +26621,7 @@
         <v>67</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>871</v>
+        <v>861</v>
       </c>
       <c r="H120" s="6"/>
     </row>
@@ -26608,7 +26639,7 @@
         <v>535</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>872</v>
+        <v>862</v>
       </c>
       <c r="H121" s="6"/>
     </row>
@@ -26680,7 +26711,7 @@
         <v>168</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>855</v>
+        <v>845</v>
       </c>
       <c r="H125" s="6"/>
     </row>
@@ -26817,7 +26848,7 @@
         <v>34</v>
       </c>
       <c r="G132" s="41" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="H132" s="20"/>
       <c r="I132" s="3"/>
@@ -26852,7 +26883,7 @@
         <v>107</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
       <c r="H133" s="6"/>
       <c r="I133" s="3"/>
@@ -27004,10 +27035,10 @@
     </row>
     <row r="138" spans="1:23" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
-        <v>867</v>
+        <v>857</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>866</v>
+        <v>856</v>
       </c>
       <c r="C138" s="7"/>
       <c r="D138" s="8"/>
@@ -27047,7 +27078,7 @@
         <v>34</v>
       </c>
       <c r="G139" s="41" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="H139" s="23"/>
       <c r="I139" s="3"/>
@@ -27082,7 +27113,7 @@
         <v>107</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>857</v>
+        <v>847</v>
       </c>
       <c r="H140" s="23"/>
       <c r="I140" s="3"/>
@@ -27115,7 +27146,7 @@
         <v>783</v>
       </c>
       <c r="G141" s="23" t="s">
-        <v>861</v>
+        <v>851</v>
       </c>
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
@@ -27147,7 +27178,7 @@
         <v>784</v>
       </c>
       <c r="G142" s="42" t="s">
-        <v>860</v>
+        <v>850</v>
       </c>
       <c r="H142" s="33"/>
       <c r="I142" s="3"/>
@@ -27180,7 +27211,7 @@
         <v>109</v>
       </c>
       <c r="G143" s="23" t="s">
-        <v>862</v>
+        <v>852</v>
       </c>
       <c r="H143" s="20"/>
       <c r="I143" s="3"/>
@@ -27213,7 +27244,7 @@
         <v>108</v>
       </c>
       <c r="G144" s="20" t="s">
-        <v>863</v>
+        <v>853</v>
       </c>
       <c r="H144" s="20"/>
       <c r="I144" s="3"/>
@@ -27237,7 +27268,7 @@
         <v>679</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>865</v>
+        <v>855</v>
       </c>
       <c r="C145" s="7"/>
       <c r="D145" s="8"/>
@@ -27277,7 +27308,7 @@
         <v>34</v>
       </c>
       <c r="G146" s="41" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="H146" s="23"/>
       <c r="I146" s="3"/>
@@ -27312,7 +27343,7 @@
         <v>107</v>
       </c>
       <c r="G147" s="6" t="s">
-        <v>857</v>
+        <v>847</v>
       </c>
       <c r="H147" s="23"/>
       <c r="I147" s="3"/>
@@ -27345,7 +27376,7 @@
         <v>783</v>
       </c>
       <c r="G148" s="23" t="s">
-        <v>870</v>
+        <v>860</v>
       </c>
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
@@ -27377,7 +27408,7 @@
         <v>784</v>
       </c>
       <c r="G149" s="42" t="s">
-        <v>868</v>
+        <v>858</v>
       </c>
       <c r="H149" s="33"/>
       <c r="I149" s="3"/>
@@ -27443,7 +27474,7 @@
         <v>108</v>
       </c>
       <c r="G151" s="23" t="s">
-        <v>869</v>
+        <v>859</v>
       </c>
       <c r="H151" s="20"/>
       <c r="I151" s="3"/>
@@ -27503,7 +27534,7 @@
         <v>200</v>
       </c>
       <c r="G153" s="42" t="s">
-        <v>956</v>
+        <v>944</v>
       </c>
       <c r="H153" s="9"/>
       <c r="I153" s="5"/>
@@ -27714,7 +27745,7 @@
         <v>209</v>
       </c>
       <c r="G160" s="33" t="s">
-        <v>955</v>
+        <v>943</v>
       </c>
       <c r="H160" s="31" t="s">
         <v>180</v>
@@ -27948,7 +27979,7 @@
         <v>429</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>873</v>
+        <v>863</v>
       </c>
       <c r="C168" s="7"/>
       <c r="D168" s="8"/>
@@ -27986,7 +28017,7 @@
         <v>756</v>
       </c>
       <c r="G169" s="42" t="s">
-        <v>876</v>
+        <v>866</v>
       </c>
       <c r="H169" s="9"/>
       <c r="I169" s="5"/>
@@ -28019,7 +28050,7 @@
         <v>34</v>
       </c>
       <c r="G170" s="20" t="s">
-        <v>877</v>
+        <v>867</v>
       </c>
       <c r="H170" s="9"/>
       <c r="I170" s="5"/>
@@ -28050,7 +28081,7 @@
         <v>430</v>
       </c>
       <c r="G171" s="20" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="H171" s="9"/>
       <c r="I171" s="5"/>
@@ -28081,7 +28112,7 @@
         <v>430</v>
       </c>
       <c r="G172" s="33" t="s">
-        <v>878</v>
+        <v>868</v>
       </c>
       <c r="H172" s="9"/>
       <c r="I172" s="5"/>
@@ -28145,7 +28176,7 @@
         <v>267</v>
       </c>
       <c r="G174" s="33" t="s">
-        <v>879</v>
+        <v>869</v>
       </c>
       <c r="H174" s="9"/>
       <c r="I174" s="5"/>
@@ -28176,7 +28207,7 @@
         <v>280</v>
       </c>
       <c r="G175" s="33" t="s">
-        <v>880</v>
+        <v>870</v>
       </c>
       <c r="H175" s="9"/>
       <c r="I175" s="5"/>
@@ -28238,7 +28269,7 @@
         <v>188</v>
       </c>
       <c r="G177" s="20" t="s">
-        <v>881</v>
+        <v>871</v>
       </c>
       <c r="H177" s="9"/>
       <c r="I177" s="5"/>
@@ -28269,7 +28300,7 @@
         <v>189</v>
       </c>
       <c r="G178" s="33" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="H178" s="9"/>
       <c r="I178" s="5"/>
@@ -28362,7 +28393,7 @@
         <v>282</v>
       </c>
       <c r="G181" s="33" t="s">
-        <v>880</v>
+        <v>870</v>
       </c>
       <c r="H181" s="9"/>
       <c r="I181" s="5"/>
@@ -28393,7 +28424,7 @@
         <v>191</v>
       </c>
       <c r="G182" s="33" t="s">
-        <v>883</v>
+        <v>873</v>
       </c>
       <c r="H182" s="9"/>
       <c r="I182" s="5"/>
@@ -28800,7 +28831,7 @@
         <v>429</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>874</v>
+        <v>864</v>
       </c>
       <c r="C195" s="7"/>
       <c r="D195" s="8"/>
@@ -28838,7 +28869,7 @@
         <v>756</v>
       </c>
       <c r="G196" s="42" t="s">
-        <v>884</v>
+        <v>874</v>
       </c>
       <c r="H196" s="9"/>
       <c r="I196" s="5"/>
@@ -28871,7 +28902,7 @@
         <v>34</v>
       </c>
       <c r="G197" s="20" t="s">
-        <v>877</v>
+        <v>867</v>
       </c>
       <c r="H197" s="9"/>
       <c r="I197" s="5"/>
@@ -28902,7 +28933,7 @@
         <v>430</v>
       </c>
       <c r="G198" s="20" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="H198" s="9"/>
       <c r="I198" s="5"/>
@@ -28933,7 +28964,7 @@
         <v>430</v>
       </c>
       <c r="G199" s="33" t="s">
-        <v>878</v>
+        <v>868</v>
       </c>
       <c r="H199" s="9"/>
       <c r="I199" s="5"/>
@@ -28997,7 +29028,7 @@
         <v>267</v>
       </c>
       <c r="G201" s="33" t="s">
-        <v>885</v>
+        <v>875</v>
       </c>
       <c r="H201" s="9"/>
       <c r="I201" s="5"/>
@@ -29028,7 +29059,7 @@
         <v>280</v>
       </c>
       <c r="G202" s="33" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
       <c r="H202" s="9"/>
       <c r="I202" s="5"/>
@@ -29090,7 +29121,7 @@
         <v>188</v>
       </c>
       <c r="G204" s="20" t="s">
-        <v>887</v>
+        <v>877</v>
       </c>
       <c r="H204" s="9"/>
       <c r="I204" s="5"/>
@@ -29121,7 +29152,7 @@
         <v>189</v>
       </c>
       <c r="G205" s="33" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="H205" s="9"/>
       <c r="I205" s="5"/>
@@ -29214,7 +29245,7 @@
         <v>282</v>
       </c>
       <c r="G208" s="33" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
       <c r="H208" s="9"/>
       <c r="I208" s="5"/>
@@ -29245,7 +29276,7 @@
         <v>191</v>
       </c>
       <c r="G209" s="33" t="s">
-        <v>883</v>
+        <v>873</v>
       </c>
       <c r="H209" s="9"/>
       <c r="I209" s="5"/>
@@ -29652,7 +29683,7 @@
         <v>429</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>875</v>
+        <v>865</v>
       </c>
       <c r="C222" s="7"/>
       <c r="D222" s="8"/>
@@ -29690,7 +29721,7 @@
         <v>756</v>
       </c>
       <c r="G223" s="42" t="s">
-        <v>888</v>
+        <v>878</v>
       </c>
       <c r="H223" s="9"/>
       <c r="I223" s="5"/>
@@ -29723,7 +29754,7 @@
         <v>34</v>
       </c>
       <c r="G224" s="20" t="s">
-        <v>877</v>
+        <v>867</v>
       </c>
       <c r="H224" s="9"/>
       <c r="I224" s="5"/>
@@ -29754,7 +29785,7 @@
         <v>430</v>
       </c>
       <c r="G225" s="20" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="H225" s="9"/>
       <c r="I225" s="5"/>
@@ -29785,7 +29816,7 @@
         <v>430</v>
       </c>
       <c r="G226" s="33" t="s">
-        <v>889</v>
+        <v>879</v>
       </c>
       <c r="H226" s="9"/>
       <c r="I226" s="5"/>
@@ -29849,7 +29880,7 @@
         <v>267</v>
       </c>
       <c r="G228" s="33" t="s">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="H228" s="9"/>
       <c r="I228" s="5"/>
@@ -29880,7 +29911,7 @@
         <v>280</v>
       </c>
       <c r="G229" s="33" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
       <c r="H229" s="9"/>
       <c r="I229" s="5"/>
@@ -29942,7 +29973,7 @@
         <v>188</v>
       </c>
       <c r="G231" s="20" t="s">
-        <v>887</v>
+        <v>877</v>
       </c>
       <c r="H231" s="9"/>
       <c r="I231" s="5"/>
@@ -29973,7 +30004,7 @@
         <v>189</v>
       </c>
       <c r="G232" s="33" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="H232" s="9"/>
       <c r="I232" s="5"/>
@@ -30066,7 +30097,7 @@
         <v>282</v>
       </c>
       <c r="G235" s="33" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
       <c r="H235" s="9"/>
       <c r="I235" s="5"/>
@@ -30097,7 +30128,7 @@
         <v>191</v>
       </c>
       <c r="G236" s="33" t="s">
-        <v>883</v>
+        <v>873</v>
       </c>
       <c r="H236" s="9"/>
       <c r="I236" s="5"/>

</xml_diff>

<commit_message>
Endret logikk for "Maks antall per fil" til å behandle "Maks antall saker"
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="2961" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84BF47CC-F967-46FA-BD4C-C9F15E06258C}"/>
   <bookViews>
-    <workbookView xWindow="4870" yWindow="2250" windowWidth="28850" windowHeight="18450" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5810" yWindow="240" windowWidth="24120" windowHeight="18510" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Fins ikke i Acos" guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Må mappes" guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Fins ikke i Acos" guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3665,7 +3665,9 @@
   </sheetPr>
   <dimension ref="A1:W949"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B393" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G403" sqref="G403"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -24797,25 +24799,25 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{B184A29A-4BF8-4FE3-9AC1-FC2281AB63EE}">
-        <filterColumn colId="5">
-          <filters blank="1">
-            <filter val="-"/>
-            <filter val="?"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{CE57DAE5-9C2E-4C88-9447-15B6A69AD455}">
+      <autoFilter ref="A1:AB1210" xr:uid="{55D46ECE-DE74-4948-B507-D12140E39F4A}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
             <filter val="Må mappes"/>
             <filter val="x"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:N83" xr:uid="{FFC62223-047D-4F95-9349-A7319F9435EC}">
+        <filterColumn colId="5">
+          <filters blank="1">
+            <filter val="-"/>
+            <filter val="?"/>
           </filters>
         </filterColumn>
       </autoFilter>

</xml_diff>

<commit_message>
Omgjort "Hent filer" til funksjonalitet for kun filuttrekk til bruk for føropplasting samt mindre justeringer.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2961" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84BF47CC-F967-46FA-BD4C-C9F15E06258C}"/>
+  <xr:revisionPtr revIDLastSave="2967" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E52804CF-6767-4410-B271-E82827C09D12}"/>
   <bookViews>
-    <workbookView xWindow="5810" yWindow="240" windowWidth="24120" windowHeight="18510" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5000" yWindow="5270" windowWidth="22240" windowHeight="13170" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -2441,9 +2441,6 @@
     <t>employee_employee.Employee_EmployeeId+BVV</t>
   </si>
   <si>
-    <t>BVV01</t>
-  </si>
-  <si>
     <t>employee_employee.FirstName + " " + MiddleName + " " + LastName</t>
   </si>
   <si>
@@ -3030,6 +3027,9 @@
   </si>
   <si>
     <t>Lovhjemmel tilknyttet vedtaket Påkrevd for Aktivitetsundertype som ikke er ADRESSESPERRE, FLYTTING, UNNDRATT_INNSYNN og alle typer Akuttvedtak</t>
+  </si>
+  <si>
+    <t>BVV1</t>
   </si>
 </sst>
 </file>
@@ -3665,9 +3665,7 @@
   </sheetPr>
   <dimension ref="A1:W949"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B393" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G403" sqref="G403"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4045,7 +4043,7 @@
         <v>564</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="12.5" x14ac:dyDescent="0.25">
@@ -4065,7 +4063,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>32</v>
@@ -4197,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>402</v>
@@ -4211,7 +4209,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>20</v>
@@ -4239,7 +4237,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G25" s="41" t="s">
         <v>415</v>
@@ -4387,13 +4385,13 @@
     </row>
     <row r="36" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="45" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>20</v>
@@ -4401,13 +4399,13 @@
     </row>
     <row r="37" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="45" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>20</v>
@@ -4421,7 +4419,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>20</v>
@@ -4461,7 +4459,7 @@
         <v>564</v>
       </c>
       <c r="G40" s="41" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -4481,7 +4479,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>733</v>
@@ -4613,7 +4611,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G48" s="41" t="s">
         <v>737</v>
@@ -4627,7 +4625,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>20</v>
@@ -4655,7 +4653,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G51" s="41" t="s">
         <v>415</v>
@@ -4803,13 +4801,13 @@
     </row>
     <row r="62" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="45" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>20</v>
@@ -4817,13 +4815,13 @@
     </row>
     <row r="63" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="45" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G63" s="6" t="s">
         <v>20</v>
@@ -4837,7 +4835,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>20</v>
@@ -4877,7 +4875,7 @@
         <v>564</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -4897,7 +4895,7 @@
         <v>50</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>32</v>
@@ -5029,7 +5027,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>402</v>
@@ -5043,7 +5041,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>20</v>
@@ -5071,7 +5069,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G77" s="41" t="s">
         <v>592</v>
@@ -5219,13 +5217,13 @@
     </row>
     <row r="88" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="45" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C88" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>20</v>
@@ -5233,13 +5231,13 @@
     </row>
     <row r="89" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="45" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C89" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>20</v>
@@ -5253,7 +5251,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>20</v>
@@ -5293,7 +5291,7 @@
         <v>564</v>
       </c>
       <c r="G92" s="41" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -5313,10 +5311,10 @@
         <v>50</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="G93" s="41" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -5339,7 +5337,7 @@
         <v>259</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="H94" s="28" t="s">
         <v>180</v>
@@ -5445,7 +5443,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>746</v>
@@ -5459,7 +5457,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>20</v>
@@ -5487,7 +5485,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G103" s="41" t="s">
         <v>748</v>
@@ -5635,13 +5633,13 @@
     </row>
     <row r="114" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="45" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C114" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G114" s="6" t="s">
         <v>20</v>
@@ -5649,13 +5647,13 @@
     </row>
     <row r="115" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="45" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C115" s="27" t="s">
         <v>1</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G115" s="6" t="s">
         <v>20</v>
@@ -5669,7 +5667,7 @@
         <v>1</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>20</v>
@@ -5712,7 +5710,7 @@
     </row>
     <row r="119" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A119" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B119" s="13" t="s">
         <v>2</v>
@@ -5721,7 +5719,7 @@
         <v>49</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="G119" s="6" t="s">
         <v>15</v>
@@ -5966,7 +5964,7 @@
         <v>5</v>
       </c>
       <c r="F135" s="6" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G135" s="6" t="s">
         <v>20</v>
@@ -6404,7 +6402,7 @@
     </row>
     <row r="166" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A166" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B166" s="13" t="s">
         <v>2</v>
@@ -6413,10 +6411,10 @@
         <v>49</v>
       </c>
       <c r="F166" s="6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="G166" s="41" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="167" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -6655,7 +6653,7 @@
         <v>5</v>
       </c>
       <c r="F182" s="6" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G182" s="6" t="s">
         <v>20</v>
@@ -7095,7 +7093,7 @@
     </row>
     <row r="213" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A213" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B213" s="13" t="s">
         <v>2</v>
@@ -7104,10 +7102,10 @@
         <v>49</v>
       </c>
       <c r="F213" s="6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="G213" s="41" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="214" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -7346,7 +7344,7 @@
         <v>5</v>
       </c>
       <c r="F229" s="6" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G229" s="41" t="s">
         <v>605</v>
@@ -7512,7 +7510,7 @@
         <v>550</v>
       </c>
       <c r="G240" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="241" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
@@ -7526,7 +7524,7 @@
         <v>407</v>
       </c>
       <c r="G241" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="242" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
@@ -7540,7 +7538,7 @@
         <v>62</v>
       </c>
       <c r="G242" s="6" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="243" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
@@ -7554,7 +7552,7 @@
         <v>63</v>
       </c>
       <c r="G243" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="244" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
@@ -7610,7 +7608,7 @@
         <v>67</v>
       </c>
       <c r="G247" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="248" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
@@ -7981,7 +7979,7 @@
         <v>550</v>
       </c>
       <c r="G272" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="273" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -7995,7 +7993,7 @@
         <v>407</v>
       </c>
       <c r="G273" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="274" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -8009,7 +8007,7 @@
         <v>62</v>
       </c>
       <c r="G274" s="6" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="275" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -8023,7 +8021,7 @@
         <v>63</v>
       </c>
       <c r="G275" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="276" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -8079,7 +8077,7 @@
         <v>67</v>
       </c>
       <c r="G279" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="280" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -8164,7 +8162,7 @@
         <v>34</v>
       </c>
       <c r="G285" s="20" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="H285" s="9"/>
     </row>
@@ -8272,7 +8270,7 @@
         <v>34</v>
       </c>
       <c r="G292" s="23" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="H292" s="9"/>
     </row>
@@ -8736,7 +8734,7 @@
         <v>205</v>
       </c>
       <c r="G310" s="42" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="H310" s="9"/>
       <c r="I310" s="5"/>
@@ -8855,7 +8853,7 @@
         <v>34</v>
       </c>
       <c r="G315" s="23" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="H315" s="27"/>
     </row>
@@ -9682,7 +9680,7 @@
         <v>34</v>
       </c>
       <c r="G367" s="20" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H367" s="9"/>
     </row>
@@ -10015,10 +10013,10 @@
         <v>1</v>
       </c>
       <c r="F387" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="G387" s="33" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H387" s="9"/>
     </row>
@@ -10147,13 +10145,13 @@
     </row>
     <row r="395" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A395" s="54" t="s">
+        <v>942</v>
+      </c>
+      <c r="C395" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F395" s="6" t="s">
         <v>943</v>
-      </c>
-      <c r="C395" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F395" s="6" t="s">
-        <v>944</v>
       </c>
       <c r="G395" s="6" t="s">
         <v>20</v>
@@ -10204,7 +10202,7 @@
         <v>34</v>
       </c>
       <c r="G398" s="42" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="H398" s="9"/>
     </row>
@@ -10231,7 +10229,7 @@
         <v>1</v>
       </c>
       <c r="F400" s="6" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G400" s="33" t="s">
         <v>693</v>
@@ -10249,7 +10247,7 @@
         <v>1</v>
       </c>
       <c r="F401" s="6" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="G401" s="33" t="s">
         <v>287</v>
@@ -10282,7 +10280,7 @@
         <v>12</v>
       </c>
       <c r="F403" s="6" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="G403" s="33" t="s">
         <v>695</v>
@@ -10297,7 +10295,7 @@
         <v>12</v>
       </c>
       <c r="F404" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="G404" s="33" t="s">
         <v>696</v>
@@ -10312,7 +10310,7 @@
         <v>1</v>
       </c>
       <c r="F405" s="6" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="G405" s="33" t="s">
         <v>288</v>
@@ -10327,7 +10325,7 @@
         <v>12</v>
       </c>
       <c r="F406" s="6" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G406" s="33" t="s">
         <v>696</v>
@@ -10387,7 +10385,7 @@
         <v>1</v>
       </c>
       <c r="F410" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="G410" s="33" t="s">
         <v>700</v>
@@ -10480,7 +10478,7 @@
         <v>222</v>
       </c>
       <c r="G416" s="33" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="H416" s="9"/>
     </row>
@@ -10621,7 +10619,7 @@
         <v>1</v>
       </c>
       <c r="F425" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="G425" s="33" t="s">
         <v>707</v>
@@ -10717,7 +10715,7 @@
         <v>34</v>
       </c>
       <c r="G431" s="33" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="H431" s="9"/>
     </row>
@@ -10831,7 +10829,7 @@
         <v>12</v>
       </c>
       <c r="F438" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="G438" s="33" t="s">
         <v>581</v>
@@ -10861,7 +10859,7 @@
         <v>12</v>
       </c>
       <c r="F440" s="6" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="G440" s="33" t="s">
         <v>582</v>
@@ -10876,7 +10874,7 @@
         <v>1</v>
       </c>
       <c r="F441" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="G441" s="33" t="s">
         <v>417</v>
@@ -10891,7 +10889,7 @@
         <v>12</v>
       </c>
       <c r="F442" s="6" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="G442" s="33" t="s">
         <v>294</v>
@@ -11019,10 +11017,10 @@
         <v>1</v>
       </c>
       <c r="F450" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="G450" s="33" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="H450" s="9"/>
     </row>
@@ -11034,10 +11032,10 @@
         <v>1</v>
       </c>
       <c r="F451" s="6" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G451" s="33" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H451" s="9"/>
     </row>
@@ -11049,10 +11047,10 @@
         <v>1</v>
       </c>
       <c r="F452" s="6" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G452" s="33" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="H452" s="9"/>
     </row>
@@ -11064,7 +11062,7 @@
         <v>1</v>
       </c>
       <c r="F453" s="6" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G453" s="33" t="s">
         <v>20</v>
@@ -11073,7 +11071,7 @@
     </row>
     <row r="454" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A454" s="45" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C454" s="16" t="s">
         <v>1</v>
@@ -11082,10 +11080,10 @@
         <v>4</v>
       </c>
       <c r="F454" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="G454" s="42" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="H454" s="9"/>
     </row>
@@ -11133,7 +11131,7 @@
         <v>554</v>
       </c>
       <c r="G457" s="23" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="H457" s="9"/>
     </row>
@@ -11148,7 +11146,7 @@
         <v>1</v>
       </c>
       <c r="F458" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="G458" s="33" t="s">
         <v>295</v>
@@ -11178,7 +11176,7 @@
         <v>1</v>
       </c>
       <c r="F460" s="6" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G460" s="33" t="s">
         <v>296</v>
@@ -11390,7 +11388,7 @@
         <v>1</v>
       </c>
       <c r="F474" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="G474" s="33" t="s">
         <v>291</v>
@@ -11405,7 +11403,7 @@
         <v>1</v>
       </c>
       <c r="F475" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="G475" s="33" t="s">
         <v>291</v>
@@ -11420,7 +11418,7 @@
         <v>1</v>
       </c>
       <c r="F476" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G476" s="33" t="s">
         <v>291</v>
@@ -11435,7 +11433,7 @@
         <v>1</v>
       </c>
       <c r="F477" s="6" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="G477" s="33" t="s">
         <v>291</v>
@@ -11450,7 +11448,7 @@
         <v>1</v>
       </c>
       <c r="F478" s="6" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="G478" s="33" t="s">
         <v>291</v>
@@ -11465,7 +11463,7 @@
         <v>1</v>
       </c>
       <c r="F479" s="6" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="G479" s="33" t="s">
         <v>291</v>
@@ -11474,13 +11472,13 @@
     </row>
     <row r="480" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A480" s="45" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C480" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F480" s="6" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="G480" s="33" t="s">
         <v>291</v>
@@ -11495,7 +11493,7 @@
         <v>1</v>
       </c>
       <c r="F481" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="G481" s="33" t="s">
         <v>291</v>
@@ -11510,7 +11508,7 @@
         <v>1</v>
       </c>
       <c r="F482" s="6" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="G482" s="33" t="s">
         <v>291</v>
@@ -11525,7 +11523,7 @@
         <v>1</v>
       </c>
       <c r="F483" s="6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="G483" s="33" t="s">
         <v>291</v>
@@ -11540,7 +11538,7 @@
         <v>1</v>
       </c>
       <c r="F484" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="G484" s="33" t="s">
         <v>291</v>
@@ -11567,7 +11565,7 @@
         <v>1</v>
       </c>
       <c r="F486" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G486" s="33" t="s">
         <v>303</v>
@@ -11582,7 +11580,7 @@
         <v>12</v>
       </c>
       <c r="F487" s="6" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="G487" s="33" t="s">
         <v>304</v>
@@ -11789,7 +11787,7 @@
         <v>1</v>
       </c>
       <c r="F501" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="G501" s="33" t="s">
         <v>20</v>
@@ -11857,7 +11855,7 @@
         <v>34</v>
       </c>
       <c r="G504" s="20" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H504" s="9"/>
       <c r="I504" s="5"/>
@@ -11909,14 +11907,14 @@
     </row>
     <row r="506" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A506" s="37" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B506" s="10"/>
       <c r="C506" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F506" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G506" s="20" t="s">
         <v>513</v>
@@ -12352,7 +12350,7 @@
         <v>1</v>
       </c>
       <c r="F520" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G520" s="20" t="s">
         <v>20</v>
@@ -12414,7 +12412,7 @@
         <v>3</v>
       </c>
       <c r="F522" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G522" s="20" t="s">
         <v>20</v>
@@ -12627,14 +12625,14 @@
     </row>
     <row r="529" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A529" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B529" s="10"/>
       <c r="C529" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F529" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G529" s="6" t="s">
         <v>20</v>
@@ -12717,7 +12715,7 @@
         <v>34</v>
       </c>
       <c r="G532" s="20" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H532" s="9"/>
       <c r="I532" s="5"/>
@@ -12769,14 +12767,14 @@
     </row>
     <row r="534" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A534" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B534" s="10"/>
       <c r="C534" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F534" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G534" s="33" t="s">
         <v>601</v>
@@ -13212,7 +13210,7 @@
         <v>1</v>
       </c>
       <c r="F548" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G548" s="20" t="s">
         <v>20</v>
@@ -13274,7 +13272,7 @@
         <v>3</v>
       </c>
       <c r="F550" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G550" s="20" t="s">
         <v>20</v>
@@ -13487,14 +13485,14 @@
     </row>
     <row r="557" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A557" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B557" s="10"/>
       <c r="C557" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F557" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G557" s="6" t="s">
         <v>20</v>
@@ -13577,7 +13575,7 @@
         <v>34</v>
       </c>
       <c r="G560" s="20" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H560" s="9"/>
       <c r="I560" s="5"/>
@@ -13598,7 +13596,7 @@
     </row>
     <row r="561" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A561" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B561" s="10"/>
       <c r="C561" s="16" t="s">
@@ -13636,7 +13634,7 @@
         <v>1</v>
       </c>
       <c r="F562" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G562" s="33" t="s">
         <v>602</v>
@@ -14072,7 +14070,7 @@
         <v>1</v>
       </c>
       <c r="F576" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G576" s="20" t="s">
         <v>20</v>
@@ -14134,7 +14132,7 @@
         <v>3</v>
       </c>
       <c r="F578" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G578" s="20" t="s">
         <v>20</v>
@@ -14347,14 +14345,14 @@
     </row>
     <row r="585" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A585" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B585" s="10"/>
       <c r="C585" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F585" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G585" s="6" t="s">
         <v>20</v>
@@ -14437,7 +14435,7 @@
         <v>34</v>
       </c>
       <c r="G588" s="33" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="H588" s="9"/>
       <c r="I588" s="5"/>
@@ -14458,7 +14456,7 @@
     </row>
     <row r="589" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A589" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B589" s="10"/>
       <c r="C589" s="16" t="s">
@@ -14496,7 +14494,7 @@
         <v>1</v>
       </c>
       <c r="F590" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G590" s="33" t="s">
         <v>602</v>
@@ -14932,7 +14930,7 @@
         <v>1</v>
       </c>
       <c r="F604" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G604" s="20" t="s">
         <v>20</v>
@@ -14994,7 +14992,7 @@
         <v>3</v>
       </c>
       <c r="F606" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G606" s="20" t="s">
         <v>20</v>
@@ -15147,14 +15145,14 @@
     </row>
     <row r="613" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A613" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B613" s="10"/>
       <c r="C613" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F613" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G613" s="6" t="s">
         <v>20</v>
@@ -15237,7 +15235,7 @@
         <v>34</v>
       </c>
       <c r="G616" s="33" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="H616" s="9"/>
       <c r="I616" s="5"/>
@@ -15258,7 +15256,7 @@
     </row>
     <row r="617" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A617" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B617" s="10"/>
       <c r="C617" s="16" t="s">
@@ -15296,7 +15294,7 @@
         <v>1</v>
       </c>
       <c r="F618" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G618" s="42" t="s">
         <v>779</v>
@@ -15732,7 +15730,7 @@
         <v>1</v>
       </c>
       <c r="F632" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G632" s="20" t="s">
         <v>20</v>
@@ -15794,7 +15792,7 @@
         <v>3</v>
       </c>
       <c r="F634" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G634" s="20" t="s">
         <v>20</v>
@@ -15947,14 +15945,14 @@
     </row>
     <row r="641" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A641" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B641" s="10"/>
       <c r="C641" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F641" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G641" s="6" t="s">
         <v>20</v>
@@ -16037,7 +16035,7 @@
         <v>34</v>
       </c>
       <c r="G644" s="33" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="H644" s="9"/>
       <c r="I644" s="5"/>
@@ -16058,7 +16056,7 @@
     </row>
     <row r="645" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A645" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B645" s="10"/>
       <c r="C645" s="16" t="s">
@@ -16096,7 +16094,7 @@
         <v>1</v>
       </c>
       <c r="F646" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G646" s="33" t="s">
         <v>602</v>
@@ -16532,7 +16530,7 @@
         <v>1</v>
       </c>
       <c r="F660" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G660" s="20" t="s">
         <v>20</v>
@@ -16594,7 +16592,7 @@
         <v>3</v>
       </c>
       <c r="F662" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G662" s="20" t="s">
         <v>20</v>
@@ -16747,14 +16745,14 @@
     </row>
     <row r="669" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A669" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B669" s="10"/>
       <c r="C669" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F669" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G669" s="6" t="s">
         <v>20</v>
@@ -16837,7 +16835,7 @@
         <v>34</v>
       </c>
       <c r="G672" s="33" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="H672" s="9"/>
       <c r="I672" s="5"/>
@@ -16858,7 +16856,7 @@
     </row>
     <row r="673" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A673" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B673" s="10"/>
       <c r="C673" s="16" t="s">
@@ -16896,10 +16894,10 @@
         <v>1</v>
       </c>
       <c r="F674" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G674" s="33" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H674" s="9"/>
       <c r="I674" s="5"/>
@@ -17332,7 +17330,7 @@
         <v>1</v>
       </c>
       <c r="F688" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G688" s="20" t="s">
         <v>20</v>
@@ -17394,7 +17392,7 @@
         <v>3</v>
       </c>
       <c r="F690" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G690" s="20" t="s">
         <v>20</v>
@@ -17547,14 +17545,14 @@
     </row>
     <row r="697" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A697" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B697" s="10"/>
       <c r="C697" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F697" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G697" s="6" t="s">
         <v>20</v>
@@ -17637,7 +17635,7 @@
         <v>34</v>
       </c>
       <c r="G700" s="20" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="H700" s="9"/>
       <c r="I700" s="5"/>
@@ -17658,7 +17656,7 @@
     </row>
     <row r="701" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A701" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B701" s="10"/>
       <c r="C701" s="16" t="s">
@@ -17696,7 +17694,7 @@
         <v>1</v>
       </c>
       <c r="F702" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G702" s="33" t="s">
         <v>781</v>
@@ -17763,7 +17761,7 @@
         <v>248</v>
       </c>
       <c r="G704" s="33" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H704" s="9"/>
       <c r="I704" s="5"/>
@@ -17794,7 +17792,7 @@
         <v>261</v>
       </c>
       <c r="G705" s="33" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="H705" s="9"/>
       <c r="I705" s="5"/>
@@ -17856,7 +17854,7 @@
         <v>187</v>
       </c>
       <c r="G707" s="20" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H707" s="9"/>
       <c r="I707" s="5"/>
@@ -17887,7 +17885,7 @@
         <v>188</v>
       </c>
       <c r="G708" s="33" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H708" s="9"/>
       <c r="I708" s="5"/>
@@ -17980,7 +17978,7 @@
         <v>263</v>
       </c>
       <c r="G711" s="33" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="H711" s="9"/>
       <c r="I711" s="5"/>
@@ -18011,7 +18009,7 @@
         <v>190</v>
       </c>
       <c r="G712" s="33" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="H712" s="9"/>
       <c r="I712" s="5"/>
@@ -18132,7 +18130,7 @@
         <v>1</v>
       </c>
       <c r="F716" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G716" s="20" t="s">
         <v>20</v>
@@ -18194,7 +18192,7 @@
         <v>3</v>
       </c>
       <c r="F718" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G718" s="20" t="s">
         <v>20</v>
@@ -18347,14 +18345,14 @@
     </row>
     <row r="725" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A725" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B725" s="10"/>
       <c r="C725" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F725" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G725" s="6" t="s">
         <v>20</v>
@@ -18381,7 +18379,7 @@
         <v>409</v>
       </c>
       <c r="B726" s="7" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C726" s="7"/>
       <c r="D726" s="8"/>
@@ -18404,7 +18402,7 @@
         <v>730</v>
       </c>
       <c r="G727" s="33" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="H727" s="9"/>
       <c r="I727" s="5"/>
@@ -18437,7 +18435,7 @@
         <v>34</v>
       </c>
       <c r="G728" s="20" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H728" s="9"/>
       <c r="I728" s="5"/>
@@ -18458,7 +18456,7 @@
     </row>
     <row r="729" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A729" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B729" s="10"/>
       <c r="C729" s="16" t="s">
@@ -18468,7 +18466,7 @@
         <v>410</v>
       </c>
       <c r="G729" s="20" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H729" s="9"/>
       <c r="I729" s="5"/>
@@ -18496,10 +18494,10 @@
         <v>1</v>
       </c>
       <c r="F730" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G730" s="33" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H730" s="9"/>
       <c r="I730" s="5"/>
@@ -18563,7 +18561,7 @@
         <v>248</v>
       </c>
       <c r="G732" s="33" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="H732" s="9"/>
       <c r="I732" s="5"/>
@@ -18594,7 +18592,7 @@
         <v>261</v>
       </c>
       <c r="G733" s="33" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H733" s="9"/>
       <c r="I733" s="5"/>
@@ -18656,7 +18654,7 @@
         <v>187</v>
       </c>
       <c r="G735" s="20" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="H735" s="9"/>
       <c r="I735" s="5"/>
@@ -18687,7 +18685,7 @@
         <v>188</v>
       </c>
       <c r="G736" s="33" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H736" s="9"/>
       <c r="I736" s="5"/>
@@ -18780,7 +18778,7 @@
         <v>263</v>
       </c>
       <c r="G739" s="33" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H739" s="9"/>
       <c r="I739" s="5"/>
@@ -18811,7 +18809,7 @@
         <v>190</v>
       </c>
       <c r="G740" s="33" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="H740" s="9"/>
       <c r="I740" s="5"/>
@@ -18932,7 +18930,7 @@
         <v>1</v>
       </c>
       <c r="F744" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G744" s="20" t="s">
         <v>20</v>
@@ -18994,7 +18992,7 @@
         <v>3</v>
       </c>
       <c r="F746" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G746" s="20" t="s">
         <v>20</v>
@@ -19147,14 +19145,14 @@
     </row>
     <row r="753" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A753" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B753" s="10"/>
       <c r="C753" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F753" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G753" s="6" t="s">
         <v>20</v>
@@ -19181,7 +19179,7 @@
         <v>409</v>
       </c>
       <c r="B754" s="7" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C754" s="7"/>
       <c r="D754" s="8"/>
@@ -19204,7 +19202,7 @@
         <v>730</v>
       </c>
       <c r="G755" s="33" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H755" s="9"/>
       <c r="I755" s="5"/>
@@ -19237,7 +19235,7 @@
         <v>34</v>
       </c>
       <c r="G756" s="20" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H756" s="9"/>
       <c r="I756" s="5"/>
@@ -19258,7 +19256,7 @@
     </row>
     <row r="757" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A757" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B757" s="10"/>
       <c r="C757" s="16" t="s">
@@ -19268,7 +19266,7 @@
         <v>410</v>
       </c>
       <c r="G757" s="20" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H757" s="9"/>
       <c r="I757" s="5"/>
@@ -19296,10 +19294,10 @@
         <v>1</v>
       </c>
       <c r="F758" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G758" s="33" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H758" s="9"/>
       <c r="I758" s="5"/>
@@ -19363,7 +19361,7 @@
         <v>248</v>
       </c>
       <c r="G760" s="33" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H760" s="9"/>
       <c r="I760" s="5"/>
@@ -19394,7 +19392,7 @@
         <v>261</v>
       </c>
       <c r="G761" s="33" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H761" s="9"/>
       <c r="I761" s="5"/>
@@ -19456,7 +19454,7 @@
         <v>187</v>
       </c>
       <c r="G763" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H763" s="9"/>
       <c r="I763" s="5"/>
@@ -19487,7 +19485,7 @@
         <v>188</v>
       </c>
       <c r="G764" s="33" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H764" s="9"/>
       <c r="I764" s="5"/>
@@ -19580,7 +19578,7 @@
         <v>263</v>
       </c>
       <c r="G767" s="33" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H767" s="9"/>
       <c r="I767" s="5"/>
@@ -19611,7 +19609,7 @@
         <v>190</v>
       </c>
       <c r="G768" s="33" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H768" s="9"/>
       <c r="I768" s="5"/>
@@ -19732,7 +19730,7 @@
         <v>1</v>
       </c>
       <c r="F772" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G772" s="20" t="s">
         <v>20</v>
@@ -19794,7 +19792,7 @@
         <v>3</v>
       </c>
       <c r="F774" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G774" s="20" t="s">
         <v>20</v>
@@ -19947,14 +19945,14 @@
     </row>
     <row r="781" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A781" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B781" s="10"/>
       <c r="C781" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F781" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G781" s="6" t="s">
         <v>20</v>
@@ -19981,7 +19979,7 @@
         <v>409</v>
       </c>
       <c r="B782" s="7" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C782" s="7"/>
       <c r="D782" s="8"/>
@@ -20036,7 +20034,7 @@
         <v>34</v>
       </c>
       <c r="G784" s="20" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="I784" s="5"/>
       <c r="J784" s="5"/>
@@ -20056,7 +20054,7 @@
     </row>
     <row r="785" spans="1:23" s="6" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A785" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B785" s="10"/>
       <c r="C785" s="16" t="s">
@@ -20066,7 +20064,7 @@
         <v>410</v>
       </c>
       <c r="G785" s="20" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H785" s="20"/>
       <c r="I785" s="5"/>
@@ -20094,10 +20092,10 @@
         <v>1</v>
       </c>
       <c r="F786" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G786" s="33" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H786" s="33"/>
       <c r="I786" s="5"/>
@@ -20280,7 +20278,7 @@
         <v>188</v>
       </c>
       <c r="G792" s="20" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I792" s="5"/>
       <c r="J792" s="5"/>
@@ -20517,7 +20515,7 @@
         <v>1</v>
       </c>
       <c r="F800" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G800" s="20" t="s">
         <v>20</v>
@@ -20577,7 +20575,7 @@
         <v>3</v>
       </c>
       <c r="F802" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G802" s="20" t="s">
         <v>20</v>
@@ -20723,14 +20721,14 @@
     </row>
     <row r="809" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A809" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B809" s="10"/>
       <c r="C809" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F809" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G809" s="6" t="s">
         <v>20</v>
@@ -20757,7 +20755,7 @@
         <v>409</v>
       </c>
       <c r="B810" s="7" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C810" s="7"/>
       <c r="D810" s="8"/>
@@ -20780,7 +20778,7 @@
         <v>730</v>
       </c>
       <c r="G811" s="33" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="H811" s="9"/>
       <c r="I811" s="5"/>
@@ -20813,7 +20811,7 @@
         <v>34</v>
       </c>
       <c r="G812" s="20" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H812" s="9"/>
       <c r="I812" s="5"/>
@@ -20844,7 +20842,7 @@
         <v>410</v>
       </c>
       <c r="G813" s="20" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="H813" s="9"/>
       <c r="I813" s="5"/>
@@ -20865,17 +20863,17 @@
     </row>
     <row r="814" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A814" s="23" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B814" s="10"/>
       <c r="C814" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F814" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G814" s="33" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H814" s="9"/>
       <c r="I814" s="5"/>
@@ -20939,7 +20937,7 @@
         <v>248</v>
       </c>
       <c r="G816" s="33" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H816" s="9"/>
       <c r="I816" s="5"/>
@@ -20970,7 +20968,7 @@
         <v>261</v>
       </c>
       <c r="G817" s="33" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H817" s="9"/>
       <c r="I817" s="5"/>
@@ -21032,7 +21030,7 @@
         <v>187</v>
       </c>
       <c r="G819" s="20" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="H819" s="9"/>
       <c r="I819" s="5"/>
@@ -21156,7 +21154,7 @@
         <v>263</v>
       </c>
       <c r="G823" s="33" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H823" s="9"/>
       <c r="I823" s="5"/>
@@ -21187,7 +21185,7 @@
         <v>190</v>
       </c>
       <c r="G824" s="33" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H824" s="9"/>
       <c r="I824" s="5"/>
@@ -21308,7 +21306,7 @@
         <v>1</v>
       </c>
       <c r="F828" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G828" s="20" t="s">
         <v>20</v>
@@ -21370,7 +21368,7 @@
         <v>3</v>
       </c>
       <c r="F830" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G830" s="20" t="s">
         <v>20</v>
@@ -21523,14 +21521,14 @@
     </row>
     <row r="837" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A837" s="23" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B837" s="10"/>
       <c r="C837" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F837" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G837" s="6" t="s">
         <v>20</v>
@@ -21557,7 +21555,7 @@
         <v>409</v>
       </c>
       <c r="B838" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C838" s="7"/>
       <c r="D838" s="8"/>
@@ -21613,7 +21611,7 @@
         <v>34</v>
       </c>
       <c r="G840" s="20" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H840" s="9"/>
       <c r="I840" s="5"/>
@@ -21665,17 +21663,17 @@
     </row>
     <row r="842" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A842" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B842" s="10"/>
       <c r="C842" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F842" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G842" s="20" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H842" s="9"/>
       <c r="I842" s="5"/>
@@ -22108,7 +22106,7 @@
         <v>1</v>
       </c>
       <c r="F856" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G856" s="20" t="s">
         <v>20</v>
@@ -22170,7 +22168,7 @@
         <v>3</v>
       </c>
       <c r="F858" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G858" s="20" t="s">
         <v>20</v>
@@ -22383,14 +22381,14 @@
     </row>
     <row r="865" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A865" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B865" s="10"/>
       <c r="C865" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F865" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G865" s="6" t="s">
         <v>20</v>
@@ -22417,7 +22415,7 @@
         <v>409</v>
       </c>
       <c r="B866" s="7" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C866" s="7"/>
       <c r="D866" s="8"/>
@@ -22440,7 +22438,7 @@
         <v>730</v>
       </c>
       <c r="G867" s="33" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="H867" s="9"/>
       <c r="I867" s="5"/>
@@ -22473,7 +22471,7 @@
         <v>34</v>
       </c>
       <c r="G868" s="20" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H868" s="9"/>
       <c r="I868" s="5"/>
@@ -22504,7 +22502,7 @@
         <v>410</v>
       </c>
       <c r="G869" s="20" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="H869" s="9"/>
       <c r="I869" s="5"/>
@@ -22525,17 +22523,17 @@
     </row>
     <row r="870" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A870" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B870" s="10"/>
       <c r="C870" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F870" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G870" s="33" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="H870" s="9"/>
       <c r="I870" s="5"/>
@@ -22599,7 +22597,7 @@
         <v>248</v>
       </c>
       <c r="G872" s="33" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H872" s="9"/>
       <c r="I872" s="5"/>
@@ -22630,7 +22628,7 @@
         <v>261</v>
       </c>
       <c r="G873" s="33" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="H873" s="9"/>
       <c r="I873" s="5"/>
@@ -22692,7 +22690,7 @@
         <v>187</v>
       </c>
       <c r="G875" s="20" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="H875" s="9"/>
       <c r="I875" s="5"/>
@@ -22723,7 +22721,7 @@
         <v>188</v>
       </c>
       <c r="G876" s="33" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="H876" s="9"/>
       <c r="I876" s="5"/>
@@ -22816,7 +22814,7 @@
         <v>263</v>
       </c>
       <c r="G879" s="33" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="H879" s="9"/>
       <c r="I879" s="5"/>
@@ -22847,7 +22845,7 @@
         <v>190</v>
       </c>
       <c r="G880" s="33" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H880" s="9"/>
       <c r="I880" s="5"/>
@@ -22968,10 +22966,10 @@
         <v>1</v>
       </c>
       <c r="F884" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G884" s="20" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="H884" s="9"/>
       <c r="I884" s="5"/>
@@ -23002,7 +23000,7 @@
         <v>192</v>
       </c>
       <c r="G885" s="20" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="H885" s="9"/>
       <c r="I885" s="5"/>
@@ -23030,10 +23028,10 @@
         <v>3</v>
       </c>
       <c r="F886" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G886" s="42" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="H886" s="9"/>
       <c r="I886" s="5"/>
@@ -23064,7 +23062,7 @@
         <v>594</v>
       </c>
       <c r="G887" s="42" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="H887" s="9"/>
       <c r="I887" s="5"/>
@@ -23183,14 +23181,14 @@
     </row>
     <row r="893" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A893" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B893" s="10"/>
       <c r="C893" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F893" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G893" s="6" t="s">
         <v>20</v>
@@ -23217,7 +23215,7 @@
         <v>409</v>
       </c>
       <c r="B894" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C894" s="7"/>
       <c r="D894" s="8"/>
@@ -23273,7 +23271,7 @@
         <v>34</v>
       </c>
       <c r="G896" s="33" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="H896" s="9"/>
       <c r="I896" s="5"/>
@@ -23304,7 +23302,7 @@
         <v>410</v>
       </c>
       <c r="G897" s="20" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H897" s="9"/>
       <c r="I897" s="5"/>
@@ -23325,17 +23323,17 @@
     </row>
     <row r="898" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A898" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B898" s="10"/>
       <c r="C898" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F898" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G898" s="20" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H898" s="9"/>
       <c r="I898" s="5"/>
@@ -23768,7 +23766,7 @@
         <v>1</v>
       </c>
       <c r="F912" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G912" s="20" t="s">
         <v>20</v>
@@ -23830,7 +23828,7 @@
         <v>3</v>
       </c>
       <c r="F914" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G914" s="20" t="s">
         <v>20</v>
@@ -23983,14 +23981,14 @@
     </row>
     <row r="921" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A921" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B921" s="10"/>
       <c r="C921" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F921" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G921" s="6" t="s">
         <v>20</v>
@@ -24119,14 +24117,14 @@
     </row>
     <row r="926" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A926" s="23" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B926" s="10"/>
       <c r="C926" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F926" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G926" s="33" t="s">
         <v>180</v>
@@ -24560,7 +24558,7 @@
         <v>1</v>
       </c>
       <c r="F940" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G940" s="20"/>
       <c r="H940" s="9"/>
@@ -24618,7 +24616,7 @@
         <v>3</v>
       </c>
       <c r="F942" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G942" s="33" t="s">
         <v>180</v>
@@ -24771,14 +24769,14 @@
     </row>
     <row r="949" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A949" s="23" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B949" s="10"/>
       <c r="C949" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F949" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="H949" s="9"/>
       <c r="I949" s="5"/>
@@ -24801,7 +24799,7 @@
   <customSheetViews>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{55D46ECE-DE74-4948-B507-D12140E39F4A}">
+      <autoFilter ref="A1:AB1210" xr:uid="{7B575E09-58C4-4A3F-A603-E9E0ACD17F7A}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
@@ -24813,7 +24811,7 @@
     </customSheetView>
     <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{FFC62223-047D-4F95-9349-A7319F9435EC}">
+      <autoFilter ref="A2:N83" xr:uid="{FC7393D0-4D29-4503-B899-6BD12A80DB84}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="-"/>
@@ -24957,7 +24955,7 @@
         <v>174</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>790</v>
+        <v>985</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -24991,7 +24989,7 @@
         <v>175</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>790</v>
+        <v>985</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -25153,7 +25151,7 @@
         <v>144</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -25217,7 +25215,7 @@
         <v>143</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>790</v>
+        <v>985</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>180</v>
@@ -25272,7 +25270,7 @@
         <v>564</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H14" s="6"/>
     </row>
@@ -25293,10 +25291,10 @@
         <v>50</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>790</v>
+        <v>985</v>
       </c>
       <c r="H15" s="6"/>
     </row>
@@ -25320,7 +25318,7 @@
         <v>259</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="H16" s="6"/>
     </row>
@@ -25342,7 +25340,7 @@
         <v>99</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H17" s="6"/>
     </row>
@@ -25360,7 +25358,7 @@
         <v>35</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H18" s="6"/>
     </row>
@@ -25378,7 +25376,7 @@
         <v>100</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H19" s="6"/>
     </row>
@@ -25400,7 +25398,7 @@
         <v>260</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="H20" s="6"/>
     </row>
@@ -25437,10 +25435,10 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="H22" s="6"/>
     </row>
@@ -25455,7 +25453,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>20</v>
@@ -25476,7 +25474,7 @@
         <v>40</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="H24" s="6"/>
     </row>
@@ -25491,10 +25489,10 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H25" s="41"/>
     </row>
@@ -25530,7 +25528,7 @@
         <v>36</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H27" s="6"/>
     </row>
@@ -25680,7 +25678,7 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="45" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="27" t="s">
@@ -25689,16 +25687,16 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G36" s="41" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="H36" s="41"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="45" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="27" t="s">
@@ -25707,10 +25705,10 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G37" s="41" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H37" s="41"/>
     </row>
@@ -25725,10 +25723,10 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="H38" s="41"/>
     </row>
@@ -25737,7 +25735,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
@@ -25766,14 +25764,14 @@
         <v>655</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>2</v>
@@ -25784,10 +25782,10 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6" t="s">
+        <v>946</v>
+      </c>
+      <c r="G41" s="41" t="s">
         <v>947</v>
-      </c>
-      <c r="G41" s="41" t="s">
-        <v>948</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -25823,7 +25821,7 @@
         <v>44</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="4"/>
@@ -25846,7 +25844,7 @@
         <v>101</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="4"/>
@@ -25865,7 +25863,7 @@
         <v>102</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="I44" s="28" t="s">
         <v>180</v>
@@ -25885,7 +25883,7 @@
         <v>103</v>
       </c>
       <c r="G45" s="41" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="4"/>
@@ -25904,7 +25902,7 @@
         <v>45</v>
       </c>
       <c r="G46" s="41" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="4"/>
@@ -25923,7 +25921,7 @@
         <v>46</v>
       </c>
       <c r="G47" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="4"/>
@@ -25942,7 +25940,7 @@
         <v>47</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="4"/>
@@ -25997,7 +25995,7 @@
         <v>148</v>
       </c>
       <c r="G51" s="41" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="4"/>
@@ -26016,7 +26014,7 @@
         <v>14</v>
       </c>
       <c r="G52" s="41" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="4"/>
@@ -26035,7 +26033,7 @@
         <v>50</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="4"/>
@@ -26107,7 +26105,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>20</v>
@@ -26166,7 +26164,7 @@
         <v>55</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I60" s="4"/>
     </row>
@@ -26257,7 +26255,7 @@
         <v>59</v>
       </c>
       <c r="G65" s="41" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="4"/>
@@ -26276,7 +26274,7 @@
         <v>60</v>
       </c>
       <c r="G66" s="41" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="4"/>
@@ -26295,7 +26293,7 @@
         <v>61</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="4"/>
@@ -26314,7 +26312,7 @@
         <v>550</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="4"/>
@@ -26333,7 +26331,7 @@
         <v>407</v>
       </c>
       <c r="G69" s="41" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="4"/>
@@ -26352,7 +26350,7 @@
         <v>62</v>
       </c>
       <c r="G70" s="41" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="4"/>
@@ -26443,7 +26441,7 @@
         <v>67</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H75" s="6"/>
       <c r="I75" s="4"/>
@@ -26462,7 +26460,7 @@
         <v>511</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="H76" s="6"/>
       <c r="I76" s="4"/>
@@ -26537,7 +26535,7 @@
         <v>565</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I80" s="28" t="s">
         <v>180</v>
@@ -26557,7 +26555,7 @@
         <v>625</v>
       </c>
       <c r="G81" s="41" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="H81" s="41"/>
       <c r="I81" s="4"/>
@@ -26641,7 +26639,7 @@
         <v>42</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
@@ -26670,13 +26668,13 @@
         <v>655</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H87" s="6"/>
     </row>
     <row r="88" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>2</v>
@@ -26687,10 +26685,10 @@
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
       <c r="F88" s="6" t="s">
+        <v>946</v>
+      </c>
+      <c r="G88" s="41" t="s">
         <v>947</v>
-      </c>
-      <c r="G88" s="41" t="s">
-        <v>948</v>
       </c>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
@@ -26726,7 +26724,7 @@
         <v>44</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H89" s="6"/>
     </row>
@@ -26748,7 +26746,7 @@
         <v>101</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H90" s="6"/>
     </row>
@@ -26766,7 +26764,7 @@
         <v>102</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="H91" s="6"/>
     </row>
@@ -26784,7 +26782,7 @@
         <v>103</v>
       </c>
       <c r="G92" s="41" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="H92" s="6"/>
     </row>
@@ -26802,7 +26800,7 @@
         <v>45</v>
       </c>
       <c r="G93" s="41" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H93" s="6"/>
     </row>
@@ -26820,7 +26818,7 @@
         <v>46</v>
       </c>
       <c r="G94" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H94" s="6"/>
     </row>
@@ -26838,7 +26836,7 @@
         <v>47</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="H95" s="6"/>
     </row>
@@ -26892,7 +26890,7 @@
         <v>148</v>
       </c>
       <c r="G98" s="41" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="H98" s="6"/>
     </row>
@@ -26910,7 +26908,7 @@
         <v>14</v>
       </c>
       <c r="G99" s="41" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="H99" s="6"/>
     </row>
@@ -26928,7 +26926,7 @@
         <v>50</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="H100" s="6"/>
     </row>
@@ -26999,10 +26997,10 @@
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
       <c r="F104" s="6" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G104" s="41" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -27055,7 +27053,7 @@
         <v>55</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H107" s="6"/>
     </row>
@@ -27145,7 +27143,7 @@
         <v>59</v>
       </c>
       <c r="G112" s="41" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="H112" s="6"/>
     </row>
@@ -27163,7 +27161,7 @@
         <v>60</v>
       </c>
       <c r="G113" s="41" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="H113" s="6"/>
     </row>
@@ -27181,7 +27179,7 @@
         <v>61</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="H114" s="6"/>
     </row>
@@ -27199,7 +27197,7 @@
         <v>550</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H115" s="6"/>
     </row>
@@ -27217,7 +27215,7 @@
         <v>407</v>
       </c>
       <c r="G116" s="41" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H116" s="6"/>
     </row>
@@ -27235,7 +27233,7 @@
         <v>62</v>
       </c>
       <c r="G117" s="41" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H117" s="6"/>
     </row>
@@ -27325,7 +27323,7 @@
         <v>67</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H122" s="6"/>
     </row>
@@ -27343,7 +27341,7 @@
         <v>511</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="H123" s="6"/>
     </row>
@@ -27415,7 +27413,7 @@
         <v>168</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H127" s="6"/>
     </row>
@@ -27552,7 +27550,7 @@
         <v>34</v>
       </c>
       <c r="G134" s="41" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H134" s="20"/>
       <c r="I134" s="3"/>
@@ -27587,7 +27585,7 @@
         <v>107</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H135" s="6"/>
       <c r="I135" s="3"/>
@@ -27739,10 +27737,10 @@
     </row>
     <row r="140" spans="1:23" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C140" s="7"/>
       <c r="D140" s="8"/>
@@ -27782,7 +27780,7 @@
         <v>34</v>
       </c>
       <c r="G141" s="41" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H141" s="23"/>
       <c r="I141" s="3"/>
@@ -27817,7 +27815,7 @@
         <v>107</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H142" s="23"/>
       <c r="I142" s="3"/>
@@ -27850,7 +27848,7 @@
         <v>757</v>
       </c>
       <c r="G143" s="23" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
@@ -27882,7 +27880,7 @@
         <v>758</v>
       </c>
       <c r="G144" s="42" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="H144" s="33"/>
       <c r="I144" s="3"/>
@@ -27915,7 +27913,7 @@
         <v>109</v>
       </c>
       <c r="G145" s="23" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="H145" s="20"/>
       <c r="I145" s="3"/>
@@ -27948,7 +27946,7 @@
         <v>108</v>
       </c>
       <c r="G146" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="H146" s="20"/>
       <c r="I146" s="3"/>
@@ -27972,7 +27970,7 @@
         <v>654</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C147" s="7"/>
       <c r="D147" s="8"/>
@@ -28012,7 +28010,7 @@
         <v>34</v>
       </c>
       <c r="G148" s="41" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H148" s="23"/>
       <c r="I148" s="3"/>
@@ -28047,7 +28045,7 @@
         <v>107</v>
       </c>
       <c r="G149" s="6" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H149" s="23"/>
       <c r="I149" s="3"/>
@@ -28080,7 +28078,7 @@
         <v>757</v>
       </c>
       <c r="G150" s="23" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
@@ -28112,7 +28110,7 @@
         <v>758</v>
       </c>
       <c r="G151" s="42" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="H151" s="33"/>
       <c r="I151" s="3"/>
@@ -28178,7 +28176,7 @@
         <v>108</v>
       </c>
       <c r="G153" s="23" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H153" s="20"/>
       <c r="I153" s="3"/>
@@ -28238,7 +28236,7 @@
         <v>197</v>
       </c>
       <c r="G155" s="42" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H155" s="9"/>
       <c r="I155" s="5"/>
@@ -28449,7 +28447,7 @@
         <v>206</v>
       </c>
       <c r="G162" s="33" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H162" s="31" t="s">
         <v>180</v>
@@ -28683,7 +28681,7 @@
         <v>409</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C170" s="7"/>
       <c r="D170" s="8"/>
@@ -28721,7 +28719,7 @@
         <v>730</v>
       </c>
       <c r="G171" s="42" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="H171" s="9"/>
       <c r="I171" s="5"/>
@@ -28754,7 +28752,7 @@
         <v>34</v>
       </c>
       <c r="G172" s="20" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="H172" s="9"/>
       <c r="I172" s="5"/>
@@ -28806,17 +28804,17 @@
     </row>
     <row r="174" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B174" s="10"/>
       <c r="C174" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F174" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G174" s="33" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="H174" s="9"/>
       <c r="I174" s="5"/>
@@ -28880,7 +28878,7 @@
         <v>248</v>
       </c>
       <c r="G176" s="33" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="H176" s="9"/>
       <c r="I176" s="5"/>
@@ -28911,7 +28909,7 @@
         <v>261</v>
       </c>
       <c r="G177" s="33" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="H177" s="9"/>
       <c r="I177" s="5"/>
@@ -28973,7 +28971,7 @@
         <v>187</v>
       </c>
       <c r="G179" s="20" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="H179" s="9"/>
       <c r="I179" s="5"/>
@@ -29004,7 +29002,7 @@
         <v>188</v>
       </c>
       <c r="G180" s="33" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H180" s="9"/>
       <c r="I180" s="5"/>
@@ -29097,7 +29095,7 @@
         <v>263</v>
       </c>
       <c r="G183" s="33" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="H183" s="9"/>
       <c r="I183" s="5"/>
@@ -29128,7 +29126,7 @@
         <v>190</v>
       </c>
       <c r="G184" s="33" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H184" s="9"/>
       <c r="I184" s="5"/>
@@ -29249,7 +29247,7 @@
         <v>1</v>
       </c>
       <c r="F188" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G188" s="6" t="s">
         <v>20</v>
@@ -29311,7 +29309,7 @@
         <v>3</v>
       </c>
       <c r="F190" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G190" s="6" t="s">
         <v>20</v>
@@ -29532,14 +29530,14 @@
     </row>
     <row r="197" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B197" s="10"/>
       <c r="C197" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F197" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G197" s="6" t="s">
         <v>20</v>
@@ -29566,7 +29564,7 @@
         <v>409</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C198" s="7"/>
       <c r="D198" s="8"/>
@@ -29604,7 +29602,7 @@
         <v>730</v>
       </c>
       <c r="G199" s="42" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="H199" s="9"/>
       <c r="I199" s="5"/>
@@ -29637,7 +29635,7 @@
         <v>34</v>
       </c>
       <c r="G200" s="20" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="H200" s="9"/>
       <c r="I200" s="5"/>
@@ -29689,17 +29687,17 @@
     </row>
     <row r="202" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B202" s="10"/>
       <c r="C202" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F202" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G202" s="33" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="H202" s="9"/>
       <c r="I202" s="5"/>
@@ -29763,7 +29761,7 @@
         <v>248</v>
       </c>
       <c r="G204" s="33" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="H204" s="9"/>
       <c r="I204" s="5"/>
@@ -29794,7 +29792,7 @@
         <v>261</v>
       </c>
       <c r="G205" s="33" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="H205" s="9"/>
       <c r="I205" s="5"/>
@@ -29856,7 +29854,7 @@
         <v>187</v>
       </c>
       <c r="G207" s="20" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="H207" s="9"/>
       <c r="I207" s="5"/>
@@ -29887,7 +29885,7 @@
         <v>188</v>
       </c>
       <c r="G208" s="33" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H208" s="9"/>
       <c r="I208" s="5"/>
@@ -29980,7 +29978,7 @@
         <v>263</v>
       </c>
       <c r="G211" s="33" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="H211" s="9"/>
       <c r="I211" s="5"/>
@@ -30011,7 +30009,7 @@
         <v>190</v>
       </c>
       <c r="G212" s="33" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H212" s="9"/>
       <c r="I212" s="5"/>
@@ -30132,7 +30130,7 @@
         <v>1</v>
       </c>
       <c r="F216" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G216" s="6" t="s">
         <v>20</v>
@@ -30194,7 +30192,7 @@
         <v>3</v>
       </c>
       <c r="F218" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G218" s="6" t="s">
         <v>20</v>
@@ -30415,14 +30413,14 @@
     </row>
     <row r="225" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B225" s="10"/>
       <c r="C225" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F225" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G225" s="6" t="s">
         <v>20</v>
@@ -30449,7 +30447,7 @@
         <v>409</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C226" s="7"/>
       <c r="D226" s="8"/>
@@ -30487,7 +30485,7 @@
         <v>730</v>
       </c>
       <c r="G227" s="42" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="H227" s="9"/>
       <c r="I227" s="5"/>
@@ -30520,7 +30518,7 @@
         <v>34</v>
       </c>
       <c r="G228" s="20" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="H228" s="9"/>
       <c r="I228" s="5"/>
@@ -30572,17 +30570,17 @@
     </row>
     <row r="230" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B230" s="10"/>
       <c r="C230" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F230" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G230" s="33" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H230" s="9"/>
       <c r="I230" s="5"/>
@@ -30646,7 +30644,7 @@
         <v>248</v>
       </c>
       <c r="G232" s="33" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="H232" s="9"/>
       <c r="I232" s="5"/>
@@ -30677,7 +30675,7 @@
         <v>261</v>
       </c>
       <c r="G233" s="33" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="H233" s="9"/>
       <c r="I233" s="5"/>
@@ -30739,7 +30737,7 @@
         <v>187</v>
       </c>
       <c r="G235" s="20" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="H235" s="9"/>
       <c r="I235" s="5"/>
@@ -30770,7 +30768,7 @@
         <v>188</v>
       </c>
       <c r="G236" s="33" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H236" s="9"/>
       <c r="I236" s="5"/>
@@ -30863,7 +30861,7 @@
         <v>263</v>
       </c>
       <c r="G239" s="33" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="H239" s="9"/>
       <c r="I239" s="5"/>
@@ -30894,7 +30892,7 @@
         <v>190</v>
       </c>
       <c r="G240" s="33" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H240" s="9"/>
       <c r="I240" s="5"/>
@@ -31015,7 +31013,7 @@
         <v>1</v>
       </c>
       <c r="F244" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G244" s="6" t="s">
         <v>20</v>
@@ -31077,7 +31075,7 @@
         <v>3</v>
       </c>
       <c r="F246" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G246" s="6" t="s">
         <v>20</v>
@@ -31298,14 +31296,14 @@
     </row>
     <row r="253" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="19" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B253" s="10"/>
       <c r="C253" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F253" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G253" s="6" t="s">
         <v>20</v>
@@ -31449,14 +31447,14 @@
     </row>
     <row r="258" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="23" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B258" s="10"/>
       <c r="C258" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F258" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G258" s="33" t="s">
         <v>180</v>
@@ -31890,7 +31888,7 @@
         <v>1</v>
       </c>
       <c r="F272" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G272" s="20"/>
       <c r="H272" s="9"/>
@@ -31948,7 +31946,7 @@
         <v>3</v>
       </c>
       <c r="F274" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G274" s="33" t="s">
         <v>180</v>
@@ -32169,14 +32167,14 @@
     </row>
     <row r="281" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" s="23" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B281" s="10"/>
       <c r="C281" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F281" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="H281" s="9"/>
       <c r="I281" s="5"/>

</xml_diff>

<commit_message>
Mer uttrekk fra tidligere bydeler, korrigering lovanvendelse ny BVL og diverse mindre justeringer.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3059" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC4E45F6-769D-4F6C-97AE-A3A94FC99499}"/>
+  <xr:revisionPtr revIDLastSave="3085" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA86CD64-66B5-42F4-B41C-F88E54696023}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="1630" windowWidth="25390" windowHeight="17820" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3320" yWindow="1760" windowWidth="26990" windowHeight="15580" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4831" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4833" uniqueCount="996">
   <si>
     <t>Format</t>
   </si>
@@ -3050,7 +3050,16 @@
     <t>FA_ENGASJEMENTSAVTALE.TIL_LOEPENR</t>
   </si>
   <si>
-    <t>FA_TILTAK.TIL_LOEPENR+&lt;BYDELSNUMMER&gt;+"TILFMF"</t>
+    <t>FA_KLIENTADRESSER.SBH_ENDRETAV</t>
+  </si>
+  <si>
+    <t>FA_KLIENTADRESSER.PAH_PASSIVISERTDATO</t>
+  </si>
+  <si>
+    <t>Flytting med fosterhjem</t>
+  </si>
+  <si>
+    <t>FA_KLIENTADRESSER.PAH_LOEPENR+&lt;BYDELSNUMMER&gt;+"FMF"</t>
   </si>
 </sst>
 </file>
@@ -3674,9 +3683,7 @@
   </sheetPr>
   <dimension ref="A1:W949"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A814" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A839" sqref="A839"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21606,7 +21613,7 @@
         <v>727</v>
       </c>
       <c r="G839" s="32" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
       <c r="H839" s="9"/>
       <c r="I839" s="5"/>
@@ -21752,7 +21759,7 @@
       <c r="W843" s="5"/>
     </row>
     <row r="844" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A844" s="22" t="s">
+      <c r="A844" s="19" t="s">
         <v>332</v>
       </c>
       <c r="B844" s="10" t="s">
@@ -21765,7 +21772,7 @@
         <v>247</v>
       </c>
       <c r="G844" s="32" t="s">
-        <v>180</v>
+        <v>993</v>
       </c>
       <c r="H844" s="9"/>
       <c r="I844" s="5"/>
@@ -21785,7 +21792,7 @@
       <c r="W844" s="5"/>
     </row>
     <row r="845" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A845" s="22" t="s">
+      <c r="A845" s="19" t="s">
         <v>312</v>
       </c>
       <c r="B845" s="10"/>
@@ -21796,7 +21803,7 @@
         <v>260</v>
       </c>
       <c r="G845" s="32" t="s">
-        <v>180</v>
+        <v>992</v>
       </c>
       <c r="H845" s="9"/>
       <c r="I845" s="5"/>
@@ -21847,7 +21854,7 @@
       <c r="W846" s="5"/>
     </row>
     <row r="847" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A847" s="22" t="s">
+      <c r="A847" s="19" t="s">
         <v>334</v>
       </c>
       <c r="B847" s="10"/>
@@ -21857,7 +21864,9 @@
       <c r="F847" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="G847" s="20"/>
+      <c r="G847" s="20" t="s">
+        <v>994</v>
+      </c>
       <c r="H847" s="9"/>
       <c r="I847" s="5"/>
       <c r="J847" s="5"/>
@@ -21876,7 +21885,7 @@
       <c r="W847" s="5"/>
     </row>
     <row r="848" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A848" s="22" t="s">
+      <c r="A848" s="19" t="s">
         <v>333</v>
       </c>
       <c r="B848" s="10"/>
@@ -21886,7 +21895,9 @@
       <c r="F848" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="G848" s="20"/>
+      <c r="G848" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="H848" s="9"/>
       <c r="I848" s="5"/>
       <c r="J848" s="5"/>
@@ -21967,7 +21978,7 @@
       <c r="W850" s="5"/>
     </row>
     <row r="851" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A851" s="22" t="s">
+      <c r="A851" s="19" t="s">
         <v>336</v>
       </c>
       <c r="B851" s="10"/>
@@ -21978,7 +21989,7 @@
         <v>262</v>
       </c>
       <c r="G851" s="32" t="s">
-        <v>180</v>
+        <v>992</v>
       </c>
       <c r="H851" s="9"/>
       <c r="I851" s="5"/>
@@ -21998,7 +22009,7 @@
       <c r="W851" s="5"/>
     </row>
     <row r="852" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A852" s="22" t="s">
+      <c r="A852" s="19" t="s">
         <v>337</v>
       </c>
       <c r="B852" s="10"/>
@@ -22009,7 +22020,7 @@
         <v>190</v>
       </c>
       <c r="G852" s="32" t="s">
-        <v>180</v>
+        <v>993</v>
       </c>
       <c r="H852" s="9"/>
       <c r="I852" s="5"/>
@@ -22029,7 +22040,7 @@
       <c r="W852" s="5"/>
     </row>
     <row r="853" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A853" s="22" t="s">
+      <c r="A853" s="19" t="s">
         <v>339</v>
       </c>
       <c r="B853" s="10"/>
@@ -22039,8 +22050,8 @@
       <c r="F853" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G853" s="32" t="s">
-        <v>180</v>
+      <c r="G853" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H853" s="9"/>
       <c r="I853" s="5"/>
@@ -22060,7 +22071,7 @@
       <c r="W853" s="5"/>
     </row>
     <row r="854" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A854" s="22" t="s">
+      <c r="A854" s="19" t="s">
         <v>340</v>
       </c>
       <c r="B854" s="10"/>
@@ -22070,8 +22081,8 @@
       <c r="F854" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="G854" s="32" t="s">
-        <v>180</v>
+      <c r="G854" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H854" s="9"/>
       <c r="I854" s="5"/>
@@ -22091,7 +22102,7 @@
       <c r="W854" s="5"/>
     </row>
     <row r="855" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A855" s="22" t="s">
+      <c r="A855" s="19" t="s">
         <v>341</v>
       </c>
       <c r="B855" s="10"/>
@@ -22101,8 +22112,8 @@
       <c r="F855" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="G855" s="32" t="s">
-        <v>180</v>
+      <c r="G855" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H855" s="9"/>
       <c r="I855" s="5"/>
@@ -22122,7 +22133,7 @@
       <c r="W855" s="5"/>
     </row>
     <row r="856" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A856" s="22" t="s">
+      <c r="A856" s="19" t="s">
         <v>342</v>
       </c>
       <c r="B856" s="10"/>
@@ -22132,8 +22143,8 @@
       <c r="F856" s="6" t="s">
         <v>952</v>
       </c>
-      <c r="G856" s="32" t="s">
-        <v>180</v>
+      <c r="G856" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H856" s="9"/>
       <c r="I856" s="5"/>
@@ -22153,7 +22164,7 @@
       <c r="W856" s="5"/>
     </row>
     <row r="857" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A857" s="22" t="s">
+      <c r="A857" s="19" t="s">
         <v>343</v>
       </c>
       <c r="B857" s="10"/>
@@ -22163,8 +22174,8 @@
       <c r="F857" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="G857" s="32" t="s">
-        <v>180</v>
+      <c r="G857" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H857" s="9"/>
       <c r="I857" s="5"/>
@@ -22184,7 +22195,7 @@
       <c r="W857" s="5"/>
     </row>
     <row r="858" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A858" s="22" t="s">
+      <c r="A858" s="19" t="s">
         <v>518</v>
       </c>
       <c r="B858" s="10"/>
@@ -22194,8 +22205,8 @@
       <c r="F858" s="6" t="s">
         <v>953</v>
       </c>
-      <c r="G858" s="32" t="s">
-        <v>180</v>
+      <c r="G858" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H858" s="9"/>
       <c r="I858" s="5"/>
@@ -22215,7 +22226,7 @@
       <c r="W858" s="5"/>
     </row>
     <row r="859" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A859" s="22" t="s">
+      <c r="A859" s="19" t="s">
         <v>592</v>
       </c>
       <c r="B859" s="10"/>
@@ -22225,8 +22236,8 @@
       <c r="F859" s="6" t="s">
         <v>593</v>
       </c>
-      <c r="G859" s="32" t="s">
-        <v>180</v>
+      <c r="G859" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H859" s="9"/>
       <c r="I859" s="5"/>
@@ -22246,7 +22257,7 @@
       <c r="W859" s="5"/>
     </row>
     <row r="860" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A860" s="22" t="s">
+      <c r="A860" s="19" t="s">
         <v>612</v>
       </c>
       <c r="B860" s="10"/>
@@ -22256,8 +22267,8 @@
       <c r="F860" s="6" t="s">
         <v>616</v>
       </c>
-      <c r="G860" s="32" t="s">
-        <v>180</v>
+      <c r="G860" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H860" s="9"/>
       <c r="I860" s="5"/>
@@ -22277,7 +22288,7 @@
       <c r="W860" s="5"/>
     </row>
     <row r="861" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A861" s="22" t="s">
+      <c r="A861" s="19" t="s">
         <v>613</v>
       </c>
       <c r="B861" s="10"/>
@@ -22287,8 +22298,8 @@
       <c r="F861" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="G861" s="32" t="s">
-        <v>180</v>
+      <c r="G861" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H861" s="9"/>
       <c r="I861" s="5"/>
@@ -22308,7 +22319,7 @@
       <c r="W861" s="5"/>
     </row>
     <row r="862" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A862" s="22" t="s">
+      <c r="A862" s="19" t="s">
         <v>614</v>
       </c>
       <c r="B862" s="10"/>
@@ -22318,8 +22329,8 @@
       <c r="F862" s="6" t="s">
         <v>618</v>
       </c>
-      <c r="G862" s="32" t="s">
-        <v>180</v>
+      <c r="G862" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H862" s="9"/>
       <c r="I862" s="5"/>
@@ -22339,7 +22350,7 @@
       <c r="W862" s="5"/>
     </row>
     <row r="863" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A863" s="22" t="s">
+      <c r="A863" s="19" t="s">
         <v>615</v>
       </c>
       <c r="B863" s="10"/>
@@ -22349,8 +22360,8 @@
       <c r="F863" s="6" t="s">
         <v>619</v>
       </c>
-      <c r="G863" s="32" t="s">
-        <v>180</v>
+      <c r="G863" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H863" s="9"/>
       <c r="I863" s="5"/>
@@ -22370,7 +22381,7 @@
       <c r="W863" s="5"/>
     </row>
     <row r="864" spans="1:23" s="6" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A864" s="22" t="s">
+      <c r="A864" s="19" t="s">
         <v>707</v>
       </c>
       <c r="B864" s="10"/>
@@ -22383,8 +22394,8 @@
       <c r="F864" s="6" t="s">
         <v>708</v>
       </c>
-      <c r="G864" s="32" t="s">
-        <v>180</v>
+      <c r="G864" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="H864" s="9"/>
       <c r="I864" s="5"/>
@@ -24902,7 +24913,7 @@
   <customSheetViews>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{D246963D-DB63-4830-A627-AF8E52AFD786}">
+      <autoFilter ref="A1:AB1210" xr:uid="{ECD43833-D708-4D6F-91E0-26FB17324C1F}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
@@ -24914,7 +24925,7 @@
     </customSheetView>
     <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{EF55330E-C321-488E-A215-5A84EFB2E046}">
+      <autoFilter ref="A2:N83" xr:uid="{27A95D3F-9D8F-4743-BBAC-A5C4FBBA90CF}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="-"/>

</xml_diff>

<commit_message>
Diverse rettelser og håndtering av data som ikke følger standarden, bl.a  uventet bruk av lovhjemler.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3118" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B75FD4A-7084-49A0-BB30-A288BCD41885}"/>
+  <xr:revisionPtr revIDLastSave="3119" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D8CC89E-280A-43F6-B33A-E0A9AD272ECD}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="1530" windowWidth="29510" windowHeight="17290" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3260" yWindow="2460" windowWidth="24060" windowHeight="13430" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -7863,7 +7863,7 @@
         <v>78</v>
       </c>
       <c r="G265" s="6" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="266" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -23161,7 +23161,7 @@
   <customSheetViews>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{7BF97D71-A215-4E0D-ACE8-FEB4987EEE60}">
+      <autoFilter ref="A1:AB1210" xr:uid="{0E9F2D77-FD22-4DDD-A4FA-7E4D4698D08D}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
@@ -23173,7 +23173,7 @@
     </customSheetView>
     <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{EA383DE3-0281-4B2C-9D03-7DA25B3C0EE1}">
+      <autoFilter ref="A2:N83" xr:uid="{5FED1160-DA6F-4E6F-A403-00287960E5F8}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="-"/>

</xml_diff>

<commit_message>
Lagt inn støtte for å kunne ta ut kun aktive eller passive saker,samt noen justeringer lover og logikk.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3186" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F13EB78A-6242-41E9-B0CA-603C33BE29DF}"/>
+  <xr:revisionPtr revIDLastSave="3187" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D0DBC3-4A0A-4DD7-9C96-3A32B44A0136}"/>
   <bookViews>
-    <workbookView xWindow="5410" yWindow="3950" windowWidth="27850" windowHeight="14780" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5550" yWindow="1860" windowWidth="26540" windowHeight="16640" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4648" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4648" uniqueCount="992">
   <si>
     <t>Format</t>
   </si>
@@ -3045,6 +3045,9 @@
   </si>
   <si>
     <t>FA_ENGASJEMENTSAVTALE.ENG_Tildato</t>
+  </si>
+  <si>
+    <t>FA_ENGASJEMENTSAVTALE.ENG_FRADATO</t>
   </si>
 </sst>
 </file>
@@ -19865,7 +19868,7 @@
         <v>246</v>
       </c>
       <c r="G779" s="32" t="s">
-        <v>894</v>
+        <v>991</v>
       </c>
       <c r="H779" s="9"/>
       <c r="I779" s="5"/>
@@ -23635,7 +23638,7 @@
   <customSheetViews>
     <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{8594B7B8-9392-48E2-908F-53BF981F2E50}">
+      <autoFilter ref="A2:N83" xr:uid="{43110C38-4384-4768-A175-241FFBB63C52}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="-"/>
@@ -23646,7 +23649,7 @@
     </customSheetView>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{63393C07-FF3C-4BE1-91D0-32CBB79301E2}">
+      <autoFilter ref="A1:AB1210" xr:uid="{D6A4CD21-2F15-41FA-87FF-2D62A9FC21C5}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>

</xml_diff>

<commit_message>
DB-skript for Migreringsdatabase innlagt, oppdatert lovbruk og mulighet for oppsplitting av passive saker i grupper.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="3187" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D0DBC3-4A0A-4DD7-9C96-3A32B44A0136}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="1860" windowWidth="26540" windowHeight="16640" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5650" yWindow="4780" windowWidth="22960" windowHeight="14630" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Fins ikke i Acos" guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Må mappes" guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Fins ikke i Acos" guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3671,7 +3671,9 @@
   </sheetPr>
   <dimension ref="A1:W906"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A496" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A509" sqref="A509"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23636,25 +23638,25 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{43110C38-4384-4768-A175-241FFBB63C52}">
-        <filterColumn colId="5">
-          <filters blank="1">
-            <filter val="-"/>
-            <filter val="?"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{D6A4CD21-2F15-41FA-87FF-2D62A9FC21C5}">
+      <autoFilter ref="A1:AB1210" xr:uid="{1F5DC10A-AC4C-4A80-B1BA-9FEC5650E2F5}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
             <filter val="Må mappes"/>
             <filter val="x"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:N83" xr:uid="{745DC531-509C-4ED1-B0F8-C533DCD6C331}">
+        <filterColumn colId="5">
+          <filters blank="1">
+            <filter val="-"/>
+            <filter val="?"/>
           </filters>
         </filterColumn>
       </autoFilter>

</xml_diff>

<commit_message>
Delt opp BVV i to deler, tatt bort en del historisk funksjonalitet og noen midre justeringer.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="3187" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D0DBC3-4A0A-4DD7-9C96-3A32B44A0136}"/>
   <bookViews>
-    <workbookView xWindow="5650" yWindow="4780" windowWidth="22960" windowHeight="14630" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3060" yWindow="5980" windowWidth="22690" windowHeight="13920" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Må mappes" guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Fins ikke i Acos" guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Må mappes" guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3671,9 +3671,7 @@
   </sheetPr>
   <dimension ref="A1:W906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A496" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A509" sqref="A509"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23638,25 +23636,25 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:N83" xr:uid="{24D5B5B7-338D-4102-88E7-93E6D09F2DFB}">
+        <filterColumn colId="5">
+          <filters blank="1">
+            <filter val="-"/>
+            <filter val="?"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{1F5DC10A-AC4C-4A80-B1BA-9FEC5650E2F5}">
+      <autoFilter ref="A1:AB1210" xr:uid="{239C294F-67BD-4569-B7EB-4151F25BF88E}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
             <filter val="Må mappes"/>
             <filter val="x"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{745DC531-509C-4ED1-B0F8-C533DCD6C331}">
-        <filterColumn colId="5">
-          <filters blank="1">
-            <filter val="-"/>
-            <filter val="?"/>
           </filters>
         </filterColumn>
       </autoFilter>

</xml_diff>

<commit_message>
Lagt til termindato for ufødte barn, satt "ukjent  person" for innbyggere uten fødselsnummer, rettet organisasjonskategorier, uttrekk ikke journalførte gjennomgangsdookumenter og tilbakemeldinger for meldinger.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3187" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93D0DBC3-4A0A-4DD7-9C96-3A32B44A0136}"/>
+  <xr:revisionPtr revIDLastSave="3189" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0908557A-4477-487C-AE64-E474847B52F5}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3060" yWindow="5980" windowWidth="22690" windowHeight="13920" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="2460" windowWidth="23870" windowHeight="17810" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Fins ikke i Acos" guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Må mappes" guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Fins ikke i Acos" guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4648" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4648" uniqueCount="993">
   <si>
     <t>Format</t>
   </si>
@@ -3048,6 +3048,9 @@
   </si>
   <si>
     <t>FA_ENGASJEMENTSAVTALE.ENG_FRADATO</t>
+  </si>
+  <si>
+    <t>FA_KLIENT.KLI_FOEDSELSDATO eller FA_MELDINGER.MEL_FOEDSELSDATO</t>
   </si>
 </sst>
 </file>
@@ -6001,7 +6004,7 @@
         <v>54</v>
       </c>
       <c r="G137" s="6" t="s">
-        <v>20</v>
+        <v>992</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
@@ -23636,25 +23639,25 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{24D5B5B7-338D-4102-88E7-93E6D09F2DFB}">
-        <filterColumn colId="5">
-          <filters blank="1">
-            <filter val="-"/>
-            <filter val="?"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{239C294F-67BD-4569-B7EB-4151F25BF88E}">
+      <autoFilter ref="A1:AB1210" xr:uid="{72E82AE9-78CD-405C-B23D-3D3397B5BA09}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
             <filter val="Må mappes"/>
             <filter val="x"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:N83" xr:uid="{0107AABA-1749-4FD6-B012-FE6EAD1AE707}">
+        <filterColumn colId="5">
+          <filters blank="1">
+            <filter val="-"/>
+            <filter val="?"/>
           </filters>
         </filterColumn>
       </autoFilter>

</xml_diff>

<commit_message>
Diverse midre endringer, spesielt knyttet tildatoer for rapportering.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="3190" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8FD69F3-0B6C-43CF-BD74-4E6ABA280658}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="4240" windowWidth="23590" windowHeight="16680" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11190" yWindow="1650" windowWidth="25830" windowHeight="18330" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -3674,7 +3674,9 @@
   </sheetPr>
   <dimension ref="A1:W906"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A536" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F570" sqref="F570"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23641,7 +23643,7 @@
   <customSheetViews>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{FCCA9261-0C09-48D5-84CE-5AE78D6C7B56}">
+      <autoFilter ref="A1:AB1210" xr:uid="{C03D6F74-04B1-4A8D-A7B6-15010EDC29A8}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
@@ -23653,7 +23655,7 @@
     </customSheetView>
     <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{18D8490A-B8ED-4893-9355-2E5647D76B74}">
+      <autoFilter ref="A2:N83" xr:uid="{8329BDF4-93E1-44A5-B58A-5C2D8CF11EBB}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="-"/>

</xml_diff>

<commit_message>
Diverse rettelser bl.a. ang. bruk av datoer og tilsynskommunenummer.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3190" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8FD69F3-0B6C-43CF-BD74-4E6ABA280658}"/>
+  <xr:revisionPtr revIDLastSave="3191" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3E2A0F0-3970-47A1-B889-82EEC83C1C64}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="1650" windowWidth="25830" windowHeight="18330" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="2350" windowWidth="27420" windowHeight="16530" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -3674,9 +3674,7 @@
   </sheetPr>
   <dimension ref="A1:W906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A536" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F570" sqref="F570"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12614,8 +12612,8 @@
       <c r="F528" s="6" t="s">
         <v>961</v>
       </c>
-      <c r="G528" s="6" t="s">
-        <v>20</v>
+      <c r="G528" s="41" t="s">
+        <v>959</v>
       </c>
       <c r="H528" s="9"/>
       <c r="I528" s="5"/>
@@ -23643,7 +23641,7 @@
   <customSheetViews>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{C03D6F74-04B1-4A8D-A7B6-15010EDC29A8}">
+      <autoFilter ref="A1:AB1210" xr:uid="{CA8C0E7E-7437-4F25-BBAB-B4B9806EE9C5}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
@@ -23655,7 +23653,7 @@
     </customSheetView>
     <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{8329BDF4-93E1-44A5-B58A-5C2D8CF11EBB}">
+      <autoFilter ref="A2:N83" xr:uid="{DACEABBA-8AB6-4404-8605-EE5A2D10F2D3}">
         <filterColumn colId="5">
           <filters blank="1">
             <filter val="-"/>

</xml_diff>

<commit_message>
Justering for når kommunenr skal settes.
</commit_message>
<xml_diff>
--- a/Migrering - mapping.xlsx
+++ b/Migrering - mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="3191" documentId="13_ncr:1_{65A9378A-81FB-4B29-8EBA-CE0D46DA555B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3E2A0F0-3970-47A1-B889-82EEC83C1C64}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="2350" windowWidth="27420" windowHeight="16530" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4720" yWindow="2910" windowWidth="22930" windowHeight="16850" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familia" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Må mappes" guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Fins ikke i Acos" guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Må mappes" guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3674,7 +3674,9 @@
   </sheetPr>
   <dimension ref="A1:W906"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23639,25 +23641,25 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:N83" xr:uid="{78FDBC45-E74A-4955-A815-A7C36F00AC4F}">
+        <filterColumn colId="5">
+          <filters blank="1">
+            <filter val="-"/>
+            <filter val="?"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{03FE5BB4-0D7C-4320-8570-17EE6485334C}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AB1210" xr:uid="{CA8C0E7E-7437-4F25-BBAB-B4B9806EE9C5}">
+      <autoFilter ref="A1:AB1210" xr:uid="{A27E99C2-E3F7-409B-9293-5E26EFA4ED76}">
         <filterColumn colId="4">
           <filters>
             <filter val="?"/>
             <filter val="Må mappes"/>
             <filter val="x"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{23FF0526-32FC-4ED2-BDF5-45E92D017C23}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:N83" xr:uid="{DACEABBA-8AB6-4404-8605-EE5A2D10F2D3}">
-        <filterColumn colId="5">
-          <filters blank="1">
-            <filter val="-"/>
-            <filter val="?"/>
           </filters>
         </filterColumn>
       </autoFilter>

</xml_diff>